<commit_message>
se modifico el archivo
</commit_message>
<xml_diff>
--- a/Guia de arboles y otras plantas nativas de Mty.xlsx
+++ b/Guia de arboles y otras plantas nativas de Mty.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uanledu-my.sharepoint.com/personal/carlos_martinezhrn_uanl_edu_mx/Documents/Documents/Github Projects/Guia-de-Arboles-y-Plantas-Nativas-de-Monterrey/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="401" documentId="8_{2025911F-8D31-4388-B950-35610A59B777}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{92B1AD90-49C1-4808-91B2-307404802116}"/>
+  <xr:revisionPtr revIDLastSave="855" documentId="8_{2025911F-8D31-4388-B950-35610A59B777}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2AA1BBFD-8AD6-407B-83F6-B3ACDA6CEA6F}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" firstSheet="8" activeTab="8" xr2:uid="{E5260BE0-913F-4F2E-A4BB-A577272EBBD7}"/>
+    <workbookView xWindow="9972" yWindow="36" windowWidth="13080" windowHeight="5148" firstSheet="8" activeTab="10" xr2:uid="{E5260BE0-913F-4F2E-A4BB-A577272EBBD7}"/>
   </bookViews>
   <sheets>
     <sheet name="Calendario de Floracion" sheetId="6" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="865" uniqueCount="283">
   <si>
     <t>Nombre Comun</t>
   </si>
@@ -434,9 +434,6 @@
     <t>Nopal de monte</t>
   </si>
   <si>
-    <t>Ocotillo</t>
-  </si>
-  <si>
     <t>Palma yuca</t>
   </si>
   <si>
@@ -464,9 +461,6 @@
     <t>Pino blanco</t>
   </si>
   <si>
-    <t>Pino teocote</t>
-  </si>
-  <si>
     <t>Sauce de rio</t>
   </si>
   <si>
@@ -587,9 +581,6 @@
     <t>No</t>
   </si>
   <si>
-    <t xml:space="preserve">"+ 150 años </t>
-  </si>
-  <si>
     <t>Drenado Lento o Drenado Medio</t>
   </si>
   <si>
@@ -738,6 +729,174 @@
   </si>
   <si>
     <t>Taxodium mucronatum</t>
+  </si>
+  <si>
+    <t>Follaje caduco o caducifilio, es decir que durante el otoño este cae. El arbol queda casi o totalmenete desprovisto de follaje, lo que le otorga un aspecto invernal</t>
+  </si>
+  <si>
+    <t>follaje semiperenne. Se trata de aquel arbol que durante el invierno pierde una cantidad significativa de follaje, lo que se aprecia a primera vsita. Sin embargo, su copa sigue proyectando cierta sombra. En ocasiones, las hojas remanentes se tiñen de un color otoñal.</t>
+  </si>
+  <si>
+    <t>Follaje que se mantiene constante en el arbol durante los doce meses del año. El color de las hojas si puede llegar a cambiar en la epoca otoñal ; sin embargo, la mayoria de las especies se mantienen verdes. En algunos arboles las hojas si se mudan, pero lo hacen de modo paulatino, lo que vuelve imperceptible el cambio</t>
+  </si>
+  <si>
+    <t>Estos arboles son recomendados para proyectos a largo plazo, donde no se requiera un efecto inmediato. Usualmente las especies de lento crecimiento son muy longevas</t>
+  </si>
+  <si>
+    <t>Estas especies pueden ser utilizadas en un proyecto de corto o mediano plazo. Si se aplica un riego constante durante los primero años, el crecimiento se puede acelerar.</t>
+  </si>
+  <si>
+    <t>las especies de rapido desarrollo son ideales para regeneracion de suelos o de ecosistemas, asi como para proyectos de corto plazo en los que se busca un efecto inmediato o muy proximo. Por lo general estas especies tienen un costo de adquisicion menor</t>
+  </si>
+  <si>
+    <t>Opuntia engelmannii y pheacantha</t>
+  </si>
+  <si>
+    <t>Ocotillo o Albarda</t>
+  </si>
+  <si>
+    <t>Fouquieria splendens</t>
+  </si>
+  <si>
+    <t>Fouquieriaceae</t>
+  </si>
+  <si>
+    <t>Yucca filifera</t>
+  </si>
+  <si>
+    <t>150+ años</t>
+  </si>
+  <si>
+    <t xml:space="preserve">150+ años </t>
+  </si>
+  <si>
+    <t>Echinocereus stramineus</t>
+  </si>
+  <si>
+    <t>Dasylirion texanum</t>
+  </si>
+  <si>
+    <t>Cordia boisseri</t>
+  </si>
+  <si>
+    <t>Boraginaceae</t>
+  </si>
+  <si>
+    <t>Lacustre o Ripario</t>
+  </si>
+  <si>
+    <t>Valle y Desierto</t>
+  </si>
+  <si>
+    <t>Acacia rigidula</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ehretia anacua </t>
+  </si>
+  <si>
+    <t>Ebenopsis ebano</t>
+  </si>
+  <si>
+    <t>Drenado Rapido a Drenado Lento</t>
+  </si>
+  <si>
+    <t>Quercus graciliformis</t>
+  </si>
+  <si>
+    <t>Quercus fusiformis</t>
+  </si>
+  <si>
+    <t>Quercus canbyi</t>
+  </si>
+  <si>
+    <t>Quercus laceyi</t>
+  </si>
+  <si>
+    <t>Ulmus crassifolia</t>
+  </si>
+  <si>
+    <t>Ulmaceae</t>
+  </si>
+  <si>
+    <t>Celtis laevigata</t>
+  </si>
+  <si>
+    <t>Juglans mollis</t>
+  </si>
+  <si>
+    <t>Juglandaceae</t>
+  </si>
+  <si>
+    <t>Valle o Montaña o Lacustre ripario</t>
+  </si>
+  <si>
+    <t>Carya illinoinensis</t>
+  </si>
+  <si>
+    <t>Sabal mexicana</t>
+  </si>
+  <si>
+    <t>Pinus pseudostrobus</t>
+  </si>
+  <si>
+    <t>Pinaceae</t>
+  </si>
+  <si>
+    <t>Pino teocote o colorado</t>
+  </si>
+  <si>
+    <t>Pinus teocote</t>
+  </si>
+  <si>
+    <t>Salix nigra</t>
+  </si>
+  <si>
+    <t>Valle y Lacuestre o ripario</t>
+  </si>
+  <si>
+    <t>30-80 años</t>
+  </si>
+  <si>
+    <t>Sargentia greggi</t>
+  </si>
+  <si>
+    <t>Rutaceae</t>
+  </si>
+  <si>
+    <t>Drenaje Medio</t>
+  </si>
+  <si>
+    <t>Diospyros texana</t>
+  </si>
+  <si>
+    <t>Ebenaceae</t>
+  </si>
+  <si>
+    <t>Drenaje Rapido a Drenaje Lento</t>
+  </si>
+  <si>
+    <t>Shopora secundiflora</t>
+  </si>
+  <si>
+    <t>Drenaje Rapido</t>
+  </si>
+  <si>
+    <t>Sideroxylon celastrinum</t>
+  </si>
+  <si>
+    <t>Sapotaceae</t>
+  </si>
+  <si>
+    <t>Cornus florida</t>
+  </si>
+  <si>
+    <t>Cornaceae</t>
+  </si>
+  <si>
+    <t>Cercis canadensis</t>
+  </si>
+  <si>
+    <t>Caesa</t>
   </si>
 </sst>
 </file>
@@ -2149,7 +2308,7 @@
   <dimension ref="A1:U13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2157,6 +2316,17 @@
     <col min="1" max="1" width="7.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
@@ -2231,6 +2401,48 @@
       <c r="B2" t="s">
         <v>108</v>
       </c>
+      <c r="C2" t="s">
+        <v>247</v>
+      </c>
+      <c r="D2" t="s">
+        <v>243</v>
+      </c>
+      <c r="E2" t="s">
+        <v>158</v>
+      </c>
+      <c r="F2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G2" t="s">
+        <v>87</v>
+      </c>
+      <c r="H2" t="s">
+        <v>183</v>
+      </c>
+      <c r="I2" t="s">
+        <v>200</v>
+      </c>
+      <c r="J2" t="s">
+        <v>97</v>
+      </c>
+      <c r="K2" t="s">
+        <v>196</v>
+      </c>
+      <c r="L2" t="s">
+        <v>196</v>
+      </c>
+      <c r="M2">
+        <v>6</v>
+      </c>
+      <c r="N2">
+        <v>6</v>
+      </c>
+      <c r="O2">
+        <v>8</v>
+      </c>
+      <c r="P2" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3">
@@ -2239,6 +2451,48 @@
       <c r="B3" t="s">
         <v>109</v>
       </c>
+      <c r="C3" t="s">
+        <v>248</v>
+      </c>
+      <c r="D3" t="s">
+        <v>207</v>
+      </c>
+      <c r="E3" t="s">
+        <v>160</v>
+      </c>
+      <c r="F3" t="s">
+        <v>83</v>
+      </c>
+      <c r="G3" t="s">
+        <v>87</v>
+      </c>
+      <c r="H3" t="s">
+        <v>160</v>
+      </c>
+      <c r="I3" t="s">
+        <v>200</v>
+      </c>
+      <c r="J3" t="s">
+        <v>249</v>
+      </c>
+      <c r="K3" t="s">
+        <v>196</v>
+      </c>
+      <c r="L3" t="s">
+        <v>196</v>
+      </c>
+      <c r="M3">
+        <v>7</v>
+      </c>
+      <c r="N3">
+        <v>6</v>
+      </c>
+      <c r="O3">
+        <v>8</v>
+      </c>
+      <c r="P3" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4">
@@ -2247,6 +2501,48 @@
       <c r="B4" t="s">
         <v>110</v>
       </c>
+      <c r="C4" t="s">
+        <v>250</v>
+      </c>
+      <c r="D4" t="s">
+        <v>182</v>
+      </c>
+      <c r="E4" t="s">
+        <v>158</v>
+      </c>
+      <c r="F4" t="s">
+        <v>82</v>
+      </c>
+      <c r="G4" t="s">
+        <v>87</v>
+      </c>
+      <c r="H4" t="s">
+        <v>163</v>
+      </c>
+      <c r="I4" t="s">
+        <v>200</v>
+      </c>
+      <c r="J4" t="s">
+        <v>184</v>
+      </c>
+      <c r="K4" t="s">
+        <v>196</v>
+      </c>
+      <c r="L4" t="s">
+        <v>181</v>
+      </c>
+      <c r="M4">
+        <v>8</v>
+      </c>
+      <c r="N4">
+        <v>8</v>
+      </c>
+      <c r="O4">
+        <v>10</v>
+      </c>
+      <c r="P4" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5">
@@ -2255,6 +2551,48 @@
       <c r="B5" t="s">
         <v>111</v>
       </c>
+      <c r="C5" t="s">
+        <v>251</v>
+      </c>
+      <c r="D5" t="s">
+        <v>182</v>
+      </c>
+      <c r="E5" t="s">
+        <v>158</v>
+      </c>
+      <c r="F5" t="s">
+        <v>82</v>
+      </c>
+      <c r="G5" t="s">
+        <v>87</v>
+      </c>
+      <c r="H5" t="s">
+        <v>163</v>
+      </c>
+      <c r="I5" t="s">
+        <v>200</v>
+      </c>
+      <c r="J5" t="s">
+        <v>97</v>
+      </c>
+      <c r="K5" t="s">
+        <v>196</v>
+      </c>
+      <c r="L5" t="s">
+        <v>181</v>
+      </c>
+      <c r="M5">
+        <v>10</v>
+      </c>
+      <c r="N5">
+        <v>12</v>
+      </c>
+      <c r="O5">
+        <v>12</v>
+      </c>
+      <c r="P5" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6">
@@ -2263,6 +2601,48 @@
       <c r="B6" t="s">
         <v>112</v>
       </c>
+      <c r="C6" t="s">
+        <v>252</v>
+      </c>
+      <c r="D6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E6" t="s">
+        <v>160</v>
+      </c>
+      <c r="F6" t="s">
+        <v>83</v>
+      </c>
+      <c r="G6" t="s">
+        <v>86</v>
+      </c>
+      <c r="H6" t="s">
+        <v>183</v>
+      </c>
+      <c r="I6" t="s">
+        <v>165</v>
+      </c>
+      <c r="J6" t="s">
+        <v>184</v>
+      </c>
+      <c r="K6" t="s">
+        <v>196</v>
+      </c>
+      <c r="L6" t="s">
+        <v>181</v>
+      </c>
+      <c r="M6">
+        <v>9</v>
+      </c>
+      <c r="N6">
+        <v>8</v>
+      </c>
+      <c r="O6">
+        <v>8</v>
+      </c>
+      <c r="P6" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7">
@@ -2271,6 +2651,48 @@
       <c r="B7" t="s">
         <v>113</v>
       </c>
+      <c r="C7" t="s">
+        <v>253</v>
+      </c>
+      <c r="D7" t="s">
+        <v>182</v>
+      </c>
+      <c r="E7" t="s">
+        <v>158</v>
+      </c>
+      <c r="F7" t="s">
+        <v>83</v>
+      </c>
+      <c r="G7" t="s">
+        <v>86</v>
+      </c>
+      <c r="H7" t="s">
+        <v>183</v>
+      </c>
+      <c r="I7" t="s">
+        <v>165</v>
+      </c>
+      <c r="J7" t="s">
+        <v>184</v>
+      </c>
+      <c r="K7" t="s">
+        <v>196</v>
+      </c>
+      <c r="L7" t="s">
+        <v>181</v>
+      </c>
+      <c r="M7">
+        <v>9</v>
+      </c>
+      <c r="N7">
+        <v>7.5</v>
+      </c>
+      <c r="O7">
+        <v>9</v>
+      </c>
+      <c r="P7" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8">
@@ -2279,6 +2701,48 @@
       <c r="B8" t="s">
         <v>114</v>
       </c>
+      <c r="C8" t="s">
+        <v>254</v>
+      </c>
+      <c r="D8" t="s">
+        <v>255</v>
+      </c>
+      <c r="E8" t="s">
+        <v>158</v>
+      </c>
+      <c r="F8" t="s">
+        <v>83</v>
+      </c>
+      <c r="G8" t="s">
+        <v>86</v>
+      </c>
+      <c r="H8" t="s">
+        <v>160</v>
+      </c>
+      <c r="I8" t="s">
+        <v>200</v>
+      </c>
+      <c r="J8" t="s">
+        <v>97</v>
+      </c>
+      <c r="K8" t="s">
+        <v>181</v>
+      </c>
+      <c r="L8" t="s">
+        <v>181</v>
+      </c>
+      <c r="M8">
+        <v>8</v>
+      </c>
+      <c r="N8">
+        <v>7</v>
+      </c>
+      <c r="O8">
+        <v>8</v>
+      </c>
+      <c r="P8" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9">
@@ -2287,10 +2751,52 @@
       <c r="B9" t="s">
         <v>115</v>
       </c>
+      <c r="C9" t="s">
+        <v>256</v>
+      </c>
+      <c r="D9" t="s">
+        <v>255</v>
+      </c>
+      <c r="E9" t="s">
+        <v>160</v>
+      </c>
+      <c r="F9" t="s">
+        <v>82</v>
+      </c>
+      <c r="G9" t="s">
+        <v>86</v>
+      </c>
+      <c r="H9" t="s">
+        <v>163</v>
+      </c>
+      <c r="I9" t="s">
+        <v>164</v>
+      </c>
+      <c r="J9" t="s">
+        <v>98</v>
+      </c>
+      <c r="K9" t="s">
+        <v>196</v>
+      </c>
+      <c r="L9" t="s">
+        <v>181</v>
+      </c>
+      <c r="M9">
+        <v>7</v>
+      </c>
+      <c r="N9">
+        <v>6</v>
+      </c>
+      <c r="O9">
+        <v>9</v>
+      </c>
+      <c r="P9" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="E10" t="s">
-        <v>77</v>
+        <v>158</v>
       </c>
       <c r="F10" t="s">
         <v>81</v>
@@ -2299,10 +2805,10 @@
         <v>85</v>
       </c>
       <c r="H10" t="s">
-        <v>89</v>
+        <v>183</v>
       </c>
       <c r="I10" t="s">
-        <v>91</v>
+        <v>164</v>
       </c>
       <c r="J10" t="s">
         <v>97</v>
@@ -2310,7 +2816,7 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="E11" t="s">
-        <v>78</v>
+        <v>160</v>
       </c>
       <c r="F11" t="s">
         <v>82</v>
@@ -2319,10 +2825,10 @@
         <v>86</v>
       </c>
       <c r="H11" t="s">
-        <v>78</v>
+        <v>160</v>
       </c>
       <c r="I11" t="s">
-        <v>92</v>
+        <v>165</v>
       </c>
       <c r="J11" t="s">
         <v>98</v>
@@ -2330,7 +2836,7 @@
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="E12" t="s">
-        <v>79</v>
+        <v>159</v>
       </c>
       <c r="F12" t="s">
         <v>83</v>
@@ -2339,10 +2845,10 @@
         <v>87</v>
       </c>
       <c r="H12" t="s">
-        <v>90</v>
+        <v>163</v>
       </c>
       <c r="I12" t="s">
-        <v>93</v>
+        <v>166</v>
       </c>
       <c r="J12" t="s">
         <v>99</v>
@@ -2350,7 +2856,7 @@
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="I13" t="s">
-        <v>94</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -2362,13 +2868,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E60A5AA-C027-4451-B966-CFECF96F6C4B}">
   <dimension ref="A1:U24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
@@ -2441,7 +2960,49 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>140</v>
+        <v>138</v>
+      </c>
+      <c r="C2" t="s">
+        <v>242</v>
+      </c>
+      <c r="D2" t="s">
+        <v>243</v>
+      </c>
+      <c r="E2" t="s">
+        <v>158</v>
+      </c>
+      <c r="F2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G2" t="s">
+        <v>87</v>
+      </c>
+      <c r="H2" t="s">
+        <v>163</v>
+      </c>
+      <c r="I2" t="s">
+        <v>245</v>
+      </c>
+      <c r="J2" t="s">
+        <v>98</v>
+      </c>
+      <c r="K2" t="s">
+        <v>196</v>
+      </c>
+      <c r="L2" t="s">
+        <v>181</v>
+      </c>
+      <c r="M2">
+        <v>4.5</v>
+      </c>
+      <c r="N2">
+        <v>4</v>
+      </c>
+      <c r="O2">
+        <v>5.5</v>
+      </c>
+      <c r="P2" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
@@ -2449,10 +3010,49 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>141</v>
+        <v>139</v>
+      </c>
+      <c r="C3" t="s">
+        <v>246</v>
       </c>
       <c r="D3" t="s">
-        <v>210</v>
+        <v>207</v>
+      </c>
+      <c r="E3" t="s">
+        <v>158</v>
+      </c>
+      <c r="F3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H3" t="s">
+        <v>160</v>
+      </c>
+      <c r="I3" t="s">
+        <v>245</v>
+      </c>
+      <c r="J3" t="s">
+        <v>97</v>
+      </c>
+      <c r="K3" t="s">
+        <v>181</v>
+      </c>
+      <c r="L3" t="s">
+        <v>196</v>
+      </c>
+      <c r="M3">
+        <v>4</v>
+      </c>
+      <c r="N3">
+        <v>3</v>
+      </c>
+      <c r="O3">
+        <v>4</v>
+      </c>
+      <c r="P3" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
@@ -2460,7 +3060,49 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>142</v>
+        <v>140</v>
+      </c>
+      <c r="C4" t="s">
+        <v>269</v>
+      </c>
+      <c r="D4" t="s">
+        <v>270</v>
+      </c>
+      <c r="E4" t="s">
+        <v>160</v>
+      </c>
+      <c r="F4" t="s">
+        <v>82</v>
+      </c>
+      <c r="G4" t="s">
+        <v>87</v>
+      </c>
+      <c r="H4" t="s">
+        <v>163</v>
+      </c>
+      <c r="I4" t="s">
+        <v>189</v>
+      </c>
+      <c r="J4" t="s">
+        <v>271</v>
+      </c>
+      <c r="K4" t="s">
+        <v>196</v>
+      </c>
+      <c r="L4" t="s">
+        <v>181</v>
+      </c>
+      <c r="M4">
+        <v>5.5</v>
+      </c>
+      <c r="N4">
+        <v>4</v>
+      </c>
+      <c r="O4">
+        <v>6</v>
+      </c>
+      <c r="P4" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.3">
@@ -2468,7 +3110,49 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>143</v>
+        <v>141</v>
+      </c>
+      <c r="C5" t="s">
+        <v>272</v>
+      </c>
+      <c r="D5" t="s">
+        <v>273</v>
+      </c>
+      <c r="E5" t="s">
+        <v>158</v>
+      </c>
+      <c r="F5" t="s">
+        <v>83</v>
+      </c>
+      <c r="G5" t="s">
+        <v>86</v>
+      </c>
+      <c r="H5" t="s">
+        <v>183</v>
+      </c>
+      <c r="I5" t="s">
+        <v>189</v>
+      </c>
+      <c r="J5" t="s">
+        <v>274</v>
+      </c>
+      <c r="K5" t="s">
+        <v>175</v>
+      </c>
+      <c r="L5" t="s">
+        <v>175</v>
+      </c>
+      <c r="M5">
+        <v>4.5</v>
+      </c>
+      <c r="N5">
+        <v>6</v>
+      </c>
+      <c r="O5">
+        <v>5</v>
+      </c>
+      <c r="P5" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.3">
@@ -2476,7 +3160,49 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>144</v>
+        <v>142</v>
+      </c>
+      <c r="C6" t="s">
+        <v>275</v>
+      </c>
+      <c r="D6" t="s">
+        <v>207</v>
+      </c>
+      <c r="E6" t="s">
+        <v>158</v>
+      </c>
+      <c r="F6" t="s">
+        <v>83</v>
+      </c>
+      <c r="G6" t="s">
+        <v>87</v>
+      </c>
+      <c r="H6" t="s">
+        <v>183</v>
+      </c>
+      <c r="I6" t="s">
+        <v>189</v>
+      </c>
+      <c r="J6" t="s">
+        <v>276</v>
+      </c>
+      <c r="K6" t="s">
+        <v>176</v>
+      </c>
+      <c r="L6" t="s">
+        <v>175</v>
+      </c>
+      <c r="M6">
+        <v>4</v>
+      </c>
+      <c r="N6">
+        <v>3</v>
+      </c>
+      <c r="O6">
+        <v>4.5</v>
+      </c>
+      <c r="P6" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.3">
@@ -2484,7 +3210,49 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>145</v>
+        <v>143</v>
+      </c>
+      <c r="C7" t="s">
+        <v>277</v>
+      </c>
+      <c r="D7" t="s">
+        <v>278</v>
+      </c>
+      <c r="E7" t="s">
+        <v>160</v>
+      </c>
+      <c r="F7" t="s">
+        <v>83</v>
+      </c>
+      <c r="G7" t="s">
+        <v>87</v>
+      </c>
+      <c r="H7" t="s">
+        <v>183</v>
+      </c>
+      <c r="I7" t="s">
+        <v>189</v>
+      </c>
+      <c r="J7" t="s">
+        <v>274</v>
+      </c>
+      <c r="K7" t="s">
+        <v>175</v>
+      </c>
+      <c r="L7" t="s">
+        <v>175</v>
+      </c>
+      <c r="M7">
+        <v>5.5</v>
+      </c>
+      <c r="N7">
+        <v>4.5</v>
+      </c>
+      <c r="O7">
+        <v>5</v>
+      </c>
+      <c r="P7" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.3">
@@ -2492,7 +3260,49 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>146</v>
+        <v>144</v>
+      </c>
+      <c r="C8" t="s">
+        <v>279</v>
+      </c>
+      <c r="D8" t="s">
+        <v>280</v>
+      </c>
+      <c r="E8" t="s">
+        <v>160</v>
+      </c>
+      <c r="F8" t="s">
+        <v>82</v>
+      </c>
+      <c r="G8" t="s">
+        <v>85</v>
+      </c>
+      <c r="H8" t="s">
+        <v>160</v>
+      </c>
+      <c r="I8" t="s">
+        <v>189</v>
+      </c>
+      <c r="J8" t="s">
+        <v>276</v>
+      </c>
+      <c r="K8" t="s">
+        <v>175</v>
+      </c>
+      <c r="L8" t="s">
+        <v>175</v>
+      </c>
+      <c r="M8">
+        <v>6</v>
+      </c>
+      <c r="N8">
+        <v>5</v>
+      </c>
+      <c r="O8">
+        <v>7</v>
+      </c>
+      <c r="P8" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.3">
@@ -2500,10 +3310,49 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>147</v>
+        <v>145</v>
+      </c>
+      <c r="C9" t="s">
+        <v>281</v>
       </c>
       <c r="D9" t="s">
-        <v>210</v>
+        <v>207</v>
+      </c>
+      <c r="E9" t="s">
+        <v>160</v>
+      </c>
+      <c r="F9" t="s">
+        <v>83</v>
+      </c>
+      <c r="G9" t="s">
+        <v>85</v>
+      </c>
+      <c r="H9" t="s">
+        <v>160</v>
+      </c>
+      <c r="I9" t="s">
+        <v>189</v>
+      </c>
+      <c r="J9" t="s">
+        <v>276</v>
+      </c>
+      <c r="K9" t="s">
+        <v>181</v>
+      </c>
+      <c r="L9" t="s">
+        <v>181</v>
+      </c>
+      <c r="M9">
+        <v>7</v>
+      </c>
+      <c r="N9">
+        <v>5.5</v>
+      </c>
+      <c r="O9">
+        <v>6</v>
+      </c>
+      <c r="P9" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.3">
@@ -2511,10 +3360,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>148</v>
+        <v>146</v>
+      </c>
+      <c r="C10" t="s">
+        <v>282</v>
       </c>
       <c r="D10" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.3">
@@ -2522,10 +3374,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D11" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.3">
@@ -2533,7 +3385,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.3">
@@ -2541,7 +3393,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.3">
@@ -2549,10 +3401,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D14" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.3">
@@ -2560,7 +3412,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.3">
@@ -2568,7 +3420,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
@@ -2576,7 +3428,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
@@ -2584,7 +3436,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
@@ -2595,7 +3447,7 @@
         <v>47</v>
       </c>
       <c r="D19" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
@@ -2608,7 +3460,7 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E21" t="s">
-        <v>77</v>
+        <v>158</v>
       </c>
       <c r="F21" t="s">
         <v>81</v>
@@ -2617,10 +3469,10 @@
         <v>85</v>
       </c>
       <c r="H21" t="s">
-        <v>89</v>
+        <v>183</v>
       </c>
       <c r="I21" t="s">
-        <v>91</v>
+        <v>164</v>
       </c>
       <c r="J21" t="s">
         <v>97</v>
@@ -2628,7 +3480,7 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E22" t="s">
-        <v>78</v>
+        <v>160</v>
       </c>
       <c r="F22" t="s">
         <v>82</v>
@@ -2637,10 +3489,10 @@
         <v>86</v>
       </c>
       <c r="H22" t="s">
-        <v>78</v>
+        <v>160</v>
       </c>
       <c r="I22" t="s">
-        <v>92</v>
+        <v>165</v>
       </c>
       <c r="J22" t="s">
         <v>98</v>
@@ -2648,7 +3500,7 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E23" t="s">
-        <v>79</v>
+        <v>159</v>
       </c>
       <c r="F23" t="s">
         <v>83</v>
@@ -2657,10 +3509,10 @@
         <v>87</v>
       </c>
       <c r="H23" t="s">
-        <v>90</v>
+        <v>163</v>
       </c>
       <c r="I23" t="s">
-        <v>93</v>
+        <v>166</v>
       </c>
       <c r="J23" t="s">
         <v>99</v>
@@ -2668,7 +3520,7 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="I24" t="s">
-        <v>94</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -2765,10 +3617,10 @@
         <v>116</v>
       </c>
       <c r="C2" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="D2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="E2" t="s">
         <v>77</v>
@@ -2783,16 +3635,16 @@
         <v>78</v>
       </c>
       <c r="I2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="J2" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="K2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="L2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="M2">
         <v>1.5</v>
@@ -2804,7 +3656,7 @@
         <v>1.5</v>
       </c>
       <c r="P2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
@@ -2815,10 +3667,10 @@
         <v>117</v>
       </c>
       <c r="C3" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="D3" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="E3" t="s">
         <v>77</v>
@@ -2833,16 +3685,16 @@
         <v>90</v>
       </c>
       <c r="I3" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="J3" t="s">
         <v>98</v>
       </c>
       <c r="K3" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="L3" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="M3">
         <v>2.5</v>
@@ -2854,7 +3706,7 @@
         <v>2</v>
       </c>
       <c r="P3" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
@@ -2865,10 +3717,10 @@
         <v>118</v>
       </c>
       <c r="C4" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="D4" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="E4" t="s">
         <v>77</v>
@@ -2883,16 +3735,16 @@
         <v>78</v>
       </c>
       <c r="I4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="J4" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="K4" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="L4" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="M4">
         <v>3</v>
@@ -2904,7 +3756,7 @@
         <v>3.5</v>
       </c>
       <c r="P4" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.3">
@@ -2915,10 +3767,10 @@
         <v>119</v>
       </c>
       <c r="C5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D5" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E5" t="s">
         <v>78</v>
@@ -2933,16 +3785,16 @@
         <v>90</v>
       </c>
       <c r="I5" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="J5" t="s">
         <v>99</v>
       </c>
       <c r="K5" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="L5" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="M5">
         <v>1</v>
@@ -2954,7 +3806,7 @@
         <v>1</v>
       </c>
       <c r="P5" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.3">
@@ -2965,10 +3817,10 @@
         <v>120</v>
       </c>
       <c r="C6" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D6" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="E6" t="s">
         <v>78</v>
@@ -2983,16 +3835,16 @@
         <v>90</v>
       </c>
       <c r="I6" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="J6" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="K6" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="L6" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="M6">
         <v>0.4</v>
@@ -3001,7 +3853,7 @@
         <v>0.3</v>
       </c>
       <c r="P6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.3">
@@ -3012,10 +3864,10 @@
         <v>121</v>
       </c>
       <c r="C7" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D7" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="E7" t="s">
         <v>77</v>
@@ -3030,19 +3882,19 @@
         <v>90</v>
       </c>
       <c r="I7" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="J7" t="s">
         <v>97</v>
       </c>
       <c r="K7" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="L7" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="P7" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.3">
@@ -3053,10 +3905,10 @@
         <v>122</v>
       </c>
       <c r="C8" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D8" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="E8" t="s">
         <v>79</v>
@@ -3071,16 +3923,16 @@
         <v>90</v>
       </c>
       <c r="I8" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="J8" t="s">
         <v>97</v>
       </c>
       <c r="K8" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="L8" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="M8">
         <v>0.7</v>
@@ -3092,7 +3944,7 @@
         <v>0.6</v>
       </c>
       <c r="P8" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.3">
@@ -3169,13 +4021,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A892B183-95B1-429D-A4A3-E6ADC63D4933}">
   <dimension ref="A1:U14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.44140625" bestFit="1" customWidth="1"/>
@@ -3263,10 +4116,10 @@
         <v>123</v>
       </c>
       <c r="C2" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="D2" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="E2" t="s">
         <v>77</v>
@@ -3281,16 +4134,16 @@
         <v>89</v>
       </c>
       <c r="I2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="J2" t="s">
         <v>97</v>
       </c>
       <c r="K2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="L2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="M2">
         <v>0.7</v>
@@ -3302,7 +4155,7 @@
         <v>1</v>
       </c>
       <c r="P2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
@@ -3313,10 +4166,10 @@
         <v>124</v>
       </c>
       <c r="C3" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="D3" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="E3" t="s">
         <v>77</v>
@@ -3331,16 +4184,16 @@
         <v>78</v>
       </c>
       <c r="I3" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="J3" t="s">
         <v>97</v>
       </c>
       <c r="K3" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="L3" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="M3">
         <v>1.5</v>
@@ -3352,7 +4205,7 @@
         <v>1.6</v>
       </c>
       <c r="P3" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
@@ -3363,10 +4216,10 @@
         <v>125</v>
       </c>
       <c r="C4" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="D4" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="E4" t="s">
         <v>77</v>
@@ -3381,16 +4234,16 @@
         <v>78</v>
       </c>
       <c r="I4" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="J4" t="s">
         <v>97</v>
       </c>
       <c r="K4" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="L4" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="M4">
         <v>0.6</v>
@@ -3402,7 +4255,7 @@
         <v>0.8</v>
       </c>
       <c r="P4" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.3">
@@ -3413,10 +4266,10 @@
         <v>126</v>
       </c>
       <c r="C5" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="D5" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="E5" t="s">
         <v>77</v>
@@ -3431,16 +4284,16 @@
         <v>90</v>
       </c>
       <c r="I5" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="J5" t="s">
         <v>97</v>
       </c>
       <c r="K5" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="L5" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="M5">
         <v>1.2</v>
@@ -3452,7 +4305,7 @@
         <v>2</v>
       </c>
       <c r="P5" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.3">
@@ -3462,8 +4315,47 @@
       <c r="B6" t="s">
         <v>127</v>
       </c>
+      <c r="C6" t="s">
+        <v>233</v>
+      </c>
+      <c r="D6" t="s">
+        <v>216</v>
+      </c>
+      <c r="E6" t="s">
+        <v>77</v>
+      </c>
+      <c r="F6" t="s">
+        <v>82</v>
+      </c>
+      <c r="G6" t="s">
+        <v>87</v>
+      </c>
+      <c r="H6" t="s">
+        <v>90</v>
+      </c>
+      <c r="I6" t="s">
+        <v>217</v>
+      </c>
+      <c r="J6" t="s">
+        <v>97</v>
+      </c>
+      <c r="K6" t="s">
+        <v>196</v>
+      </c>
+      <c r="L6" t="s">
+        <v>181</v>
+      </c>
+      <c r="M6">
+        <v>1.5</v>
+      </c>
+      <c r="N6">
+        <v>1.5</v>
+      </c>
+      <c r="O6">
+        <v>1.5</v>
+      </c>
       <c r="P6" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.3">
@@ -3471,7 +4363,49 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>128</v>
+        <v>234</v>
+      </c>
+      <c r="C7" t="s">
+        <v>235</v>
+      </c>
+      <c r="D7" t="s">
+        <v>236</v>
+      </c>
+      <c r="E7" t="s">
+        <v>77</v>
+      </c>
+      <c r="F7" t="s">
+        <v>82</v>
+      </c>
+      <c r="G7" t="s">
+        <v>85</v>
+      </c>
+      <c r="H7" t="s">
+        <v>78</v>
+      </c>
+      <c r="I7" t="s">
+        <v>217</v>
+      </c>
+      <c r="J7" t="s">
+        <v>97</v>
+      </c>
+      <c r="K7" t="s">
+        <v>196</v>
+      </c>
+      <c r="L7" t="s">
+        <v>181</v>
+      </c>
+      <c r="M7">
+        <v>2</v>
+      </c>
+      <c r="N7">
+        <v>1.8</v>
+      </c>
+      <c r="O7">
+        <v>2.5</v>
+      </c>
+      <c r="P7" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.3">
@@ -3479,10 +4413,49 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>129</v>
+        <v>128</v>
+      </c>
+      <c r="C8" t="s">
+        <v>237</v>
       </c>
       <c r="D8" t="s">
-        <v>226</v>
+        <v>223</v>
+      </c>
+      <c r="E8" t="s">
+        <v>77</v>
+      </c>
+      <c r="F8" t="s">
+        <v>82</v>
+      </c>
+      <c r="G8" t="s">
+        <v>87</v>
+      </c>
+      <c r="H8" t="s">
+        <v>89</v>
+      </c>
+      <c r="I8" t="s">
+        <v>217</v>
+      </c>
+      <c r="J8" t="s">
+        <v>97</v>
+      </c>
+      <c r="K8" t="s">
+        <v>181</v>
+      </c>
+      <c r="L8" t="s">
+        <v>181</v>
+      </c>
+      <c r="M8">
+        <v>4.5</v>
+      </c>
+      <c r="N8">
+        <v>3.5</v>
+      </c>
+      <c r="O8">
+        <v>4</v>
+      </c>
+      <c r="P8" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.3">
@@ -3490,7 +4463,49 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>130</v>
+        <v>129</v>
+      </c>
+      <c r="C9" t="s">
+        <v>240</v>
+      </c>
+      <c r="D9" t="s">
+        <v>216</v>
+      </c>
+      <c r="E9" t="s">
+        <v>77</v>
+      </c>
+      <c r="F9" t="s">
+        <v>81</v>
+      </c>
+      <c r="G9" t="s">
+        <v>87</v>
+      </c>
+      <c r="H9" t="s">
+        <v>78</v>
+      </c>
+      <c r="I9" t="s">
+        <v>217</v>
+      </c>
+      <c r="J9" t="s">
+        <v>97</v>
+      </c>
+      <c r="K9" t="s">
+        <v>181</v>
+      </c>
+      <c r="L9" t="s">
+        <v>181</v>
+      </c>
+      <c r="M9">
+        <v>0.4</v>
+      </c>
+      <c r="N9">
+        <v>0.8</v>
+      </c>
+      <c r="O9">
+        <v>1</v>
+      </c>
+      <c r="P9" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.3">
@@ -3498,10 +4513,49 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>131</v>
+        <v>130</v>
+      </c>
+      <c r="C10" t="s">
+        <v>241</v>
       </c>
       <c r="D10" t="s">
-        <v>226</v>
+        <v>223</v>
+      </c>
+      <c r="E10" t="s">
+        <v>77</v>
+      </c>
+      <c r="F10" t="s">
+        <v>82</v>
+      </c>
+      <c r="G10" t="s">
+        <v>87</v>
+      </c>
+      <c r="H10" t="s">
+        <v>90</v>
+      </c>
+      <c r="I10" t="s">
+        <v>217</v>
+      </c>
+      <c r="J10" t="s">
+        <v>97</v>
+      </c>
+      <c r="K10" t="s">
+        <v>181</v>
+      </c>
+      <c r="L10" t="s">
+        <v>181</v>
+      </c>
+      <c r="M10">
+        <v>0.8</v>
+      </c>
+      <c r="N10">
+        <v>1.3</v>
+      </c>
+      <c r="O10">
+        <v>1.3</v>
+      </c>
+      <c r="P10" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.3">
@@ -3579,7 +4633,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3591,13 +4645,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C1" t="s">
         <v>157</v>
-      </c>
-      <c r="B1" t="s">
-        <v>158</v>
-      </c>
-      <c r="C1" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
@@ -3605,10 +4659,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
@@ -3616,10 +4670,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="72" x14ac:dyDescent="0.3">
@@ -3627,10 +4681,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -3643,7 +4697,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C4"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3655,13 +4709,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C1" t="s">
         <v>157</v>
-      </c>
-      <c r="B1" t="s">
-        <v>158</v>
-      </c>
-      <c r="C1" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
@@ -3672,7 +4726,7 @@
         <v>81</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
@@ -3683,7 +4737,7 @@
         <v>82</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
@@ -3694,7 +4748,7 @@
         <v>83</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -3707,48 +4761,58 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="51.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C1" t="s">
         <v>157</v>
       </c>
-      <c r="B1" t="s">
-        <v>158</v>
-      </c>
-      <c r="C1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C2" s="10" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="72" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C3" s="10" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>163</v>
+        <v>161</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>229</v>
       </c>
     </row>
   </sheetData>
@@ -3761,48 +4825,58 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C1" t="s">
         <v>157</v>
       </c>
-      <c r="B1" t="s">
-        <v>158</v>
-      </c>
-      <c r="C1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+        <v>162</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+        <v>160</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>165</v>
+        <v>163</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>232</v>
       </c>
     </row>
   </sheetData>
@@ -3826,13 +4900,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C1" t="s">
         <v>157</v>
-      </c>
-      <c r="B1" t="s">
-        <v>158</v>
-      </c>
-      <c r="C1" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -3840,7 +4914,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -3848,7 +4922,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -3856,7 +4930,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -3864,7 +4938,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -3881,16 +4955,20 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.77734375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C1" t="s">
         <v>157</v>
-      </c>
-      <c r="B1" t="s">
-        <v>158</v>
-      </c>
-      <c r="C1" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -3934,13 +5012,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C1" t="s">
         <v>157</v>
-      </c>
-      <c r="B1" t="s">
-        <v>217</v>
-      </c>
-      <c r="C1" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -3967,13 +5045,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC219292-3949-4AA0-84E7-7F151D5D8C5B}">
   <dimension ref="A1:U17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.33203125" customWidth="1"/>
     <col min="2" max="2" width="22.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.88671875" bestFit="1" customWidth="1"/>
@@ -4063,16 +5139,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C2" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="D2" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="E2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F2" t="s">
         <v>81</v>
@@ -4081,19 +5157,19 @@
         <v>86</v>
       </c>
       <c r="H2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="I2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="J2" t="s">
         <v>99</v>
       </c>
       <c r="K2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="L2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="M2">
         <v>20</v>
@@ -4105,7 +5181,7 @@
         <v>20</v>
       </c>
       <c r="P2" t="s">
-        <v>179</v>
+        <v>239</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
@@ -4116,13 +5192,13 @@
         <v>65</v>
       </c>
       <c r="C3" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D3" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F3" t="s">
         <v>81</v>
@@ -4131,19 +5207,19 @@
         <v>86</v>
       </c>
       <c r="H3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="I3" t="s">
+        <v>174</v>
+      </c>
+      <c r="J3" t="s">
+        <v>177</v>
+      </c>
+      <c r="K3" t="s">
+        <v>175</v>
+      </c>
+      <c r="L3" t="s">
         <v>176</v>
-      </c>
-      <c r="J3" t="s">
-        <v>180</v>
-      </c>
-      <c r="K3" t="s">
-        <v>177</v>
-      </c>
-      <c r="L3" t="s">
-        <v>178</v>
       </c>
       <c r="M3">
         <v>20</v>
@@ -4155,7 +5231,7 @@
         <v>20</v>
       </c>
       <c r="P3" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
@@ -4163,16 +5239,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C4" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="D4" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F4" t="s">
         <v>83</v>
@@ -4181,19 +5257,19 @@
         <v>86</v>
       </c>
       <c r="H4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="I4" t="s">
+        <v>174</v>
+      </c>
+      <c r="J4" t="s">
+        <v>177</v>
+      </c>
+      <c r="K4" t="s">
         <v>176</v>
       </c>
-      <c r="J4" t="s">
-        <v>180</v>
-      </c>
-      <c r="K4" t="s">
-        <v>178</v>
-      </c>
       <c r="L4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="M4">
         <v>20</v>
@@ -4205,7 +5281,7 @@
         <v>15</v>
       </c>
       <c r="P4" t="s">
-        <v>179</v>
+        <v>239</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.3">
@@ -4213,16 +5289,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C5" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D5" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F5" t="s">
         <v>83</v>
@@ -4231,19 +5307,19 @@
         <v>86</v>
       </c>
       <c r="H5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I5" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="J5" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="K5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="L5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="M5">
         <v>20</v>
@@ -4255,7 +5331,7 @@
         <v>12</v>
       </c>
       <c r="P5" t="s">
-        <v>179</v>
+        <v>239</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.3">
@@ -4266,13 +5342,13 @@
         <v>68</v>
       </c>
       <c r="C6" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D6" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F6" t="s">
         <v>83</v>
@@ -4281,19 +5357,19 @@
         <v>87</v>
       </c>
       <c r="H6" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="I6" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="J6" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="K6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="L6" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="M6">
         <v>14</v>
@@ -4305,7 +5381,7 @@
         <v>10</v>
       </c>
       <c r="P6" t="s">
-        <v>179</v>
+        <v>239</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.3">
@@ -4316,13 +5392,13 @@
         <v>69</v>
       </c>
       <c r="C7" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D7" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E7" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F7" t="s">
         <v>82</v>
@@ -4331,19 +5407,19 @@
         <v>87</v>
       </c>
       <c r="H7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="I7" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="J7" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="K7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="L7" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="M7">
         <v>12</v>
@@ -4355,7 +5431,7 @@
         <v>12</v>
       </c>
       <c r="P7" t="s">
-        <v>179</v>
+        <v>239</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.3">
@@ -4365,13 +5441,94 @@
       <c r="B8" t="s">
         <v>16</v>
       </c>
+      <c r="C8" t="s">
+        <v>257</v>
+      </c>
+      <c r="D8" t="s">
+        <v>258</v>
+      </c>
+      <c r="E8" t="s">
+        <v>159</v>
+      </c>
+      <c r="F8" t="s">
+        <v>81</v>
+      </c>
+      <c r="G8" t="s">
+        <v>85</v>
+      </c>
+      <c r="H8" t="s">
+        <v>160</v>
+      </c>
+      <c r="I8" t="s">
+        <v>259</v>
+      </c>
+      <c r="K8" t="s">
+        <v>175</v>
+      </c>
+      <c r="L8" t="s">
+        <v>175</v>
+      </c>
+      <c r="M8">
+        <v>15</v>
+      </c>
+      <c r="N8">
+        <v>12</v>
+      </c>
+      <c r="O8">
+        <v>12</v>
+      </c>
+      <c r="P8" t="s">
+        <v>239</v>
+      </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>135</v>
+        <v>134</v>
+      </c>
+      <c r="C9" t="s">
+        <v>260</v>
+      </c>
+      <c r="D9" t="s">
+        <v>258</v>
+      </c>
+      <c r="E9" t="s">
+        <v>159</v>
+      </c>
+      <c r="F9" t="s">
+        <v>82</v>
+      </c>
+      <c r="G9" t="s">
+        <v>85</v>
+      </c>
+      <c r="H9" t="s">
+        <v>160</v>
+      </c>
+      <c r="I9" t="s">
+        <v>174</v>
+      </c>
+      <c r="J9" t="s">
+        <v>177</v>
+      </c>
+      <c r="K9" t="s">
+        <v>175</v>
+      </c>
+      <c r="L9" t="s">
+        <v>181</v>
+      </c>
+      <c r="M9">
+        <v>15</v>
+      </c>
+      <c r="N9">
+        <v>12</v>
+      </c>
+      <c r="O9">
+        <v>14</v>
+      </c>
+      <c r="P9" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.3">
@@ -4379,13 +5536,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>136</v>
+        <v>135</v>
+      </c>
+      <c r="C10" t="s">
+        <v>261</v>
       </c>
       <c r="D10" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="E10" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F10" t="s">
         <v>82</v>
@@ -4394,19 +5554,19 @@
         <v>87</v>
       </c>
       <c r="H10" t="s">
+        <v>162</v>
+      </c>
+      <c r="I10" t="s">
         <v>164</v>
-      </c>
-      <c r="I10" t="s">
-        <v>166</v>
       </c>
       <c r="J10" t="s">
         <v>98</v>
       </c>
       <c r="K10" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="L10" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="M10">
         <v>12</v>
@@ -4418,7 +5578,7 @@
         <v>8</v>
       </c>
       <c r="P10" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.3">
@@ -4426,7 +5586,49 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>137</v>
+        <v>136</v>
+      </c>
+      <c r="C11" t="s">
+        <v>262</v>
+      </c>
+      <c r="D11" t="s">
+        <v>263</v>
+      </c>
+      <c r="E11" t="s">
+        <v>160</v>
+      </c>
+      <c r="F11" t="s">
+        <v>83</v>
+      </c>
+      <c r="G11" t="s">
+        <v>87</v>
+      </c>
+      <c r="H11" t="s">
+        <v>163</v>
+      </c>
+      <c r="I11" t="s">
+        <v>165</v>
+      </c>
+      <c r="J11" t="s">
+        <v>177</v>
+      </c>
+      <c r="K11" t="s">
+        <v>175</v>
+      </c>
+      <c r="L11" t="s">
+        <v>181</v>
+      </c>
+      <c r="M11">
+        <v>15</v>
+      </c>
+      <c r="N11">
+        <v>8</v>
+      </c>
+      <c r="O11">
+        <v>10</v>
+      </c>
+      <c r="P11" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.3">
@@ -4434,7 +5636,49 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>138</v>
+        <v>264</v>
+      </c>
+      <c r="C12" t="s">
+        <v>265</v>
+      </c>
+      <c r="D12" t="s">
+        <v>263</v>
+      </c>
+      <c r="E12" t="s">
+        <v>160</v>
+      </c>
+      <c r="F12" t="s">
+        <v>83</v>
+      </c>
+      <c r="G12" t="s">
+        <v>87</v>
+      </c>
+      <c r="H12" t="s">
+        <v>160</v>
+      </c>
+      <c r="I12" t="s">
+        <v>165</v>
+      </c>
+      <c r="J12" t="s">
+        <v>177</v>
+      </c>
+      <c r="K12" t="s">
+        <v>175</v>
+      </c>
+      <c r="L12" t="s">
+        <v>176</v>
+      </c>
+      <c r="M12">
+        <v>13</v>
+      </c>
+      <c r="N12">
+        <v>7</v>
+      </c>
+      <c r="O12">
+        <v>9</v>
+      </c>
+      <c r="P12" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.3">
@@ -4442,12 +5686,54 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>139</v>
+        <v>137</v>
+      </c>
+      <c r="C13" t="s">
+        <v>266</v>
+      </c>
+      <c r="D13" t="s">
+        <v>179</v>
+      </c>
+      <c r="E13" t="s">
+        <v>159</v>
+      </c>
+      <c r="F13" t="s">
+        <v>81</v>
+      </c>
+      <c r="G13" t="s">
+        <v>86</v>
+      </c>
+      <c r="H13" t="s">
+        <v>163</v>
+      </c>
+      <c r="I13" t="s">
+        <v>267</v>
+      </c>
+      <c r="J13" t="s">
+        <v>99</v>
+      </c>
+      <c r="K13" t="s">
+        <v>176</v>
+      </c>
+      <c r="L13" t="s">
+        <v>175</v>
+      </c>
+      <c r="M13">
+        <v>15</v>
+      </c>
+      <c r="N13">
+        <v>15</v>
+      </c>
+      <c r="O13">
+        <v>20</v>
+      </c>
+      <c r="P13" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="E14" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F14" t="s">
         <v>81</v>
@@ -4456,10 +5742,10 @@
         <v>85</v>
       </c>
       <c r="H14" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="I14" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="J14" t="s">
         <v>97</v>
@@ -4467,7 +5753,7 @@
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="E15" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F15" t="s">
         <v>82</v>
@@ -4476,10 +5762,10 @@
         <v>86</v>
       </c>
       <c r="H15" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I15" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="J15" t="s">
         <v>98</v>
@@ -4487,7 +5773,7 @@
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="E16" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F16" t="s">
         <v>83</v>
@@ -4496,10 +5782,10 @@
         <v>87</v>
       </c>
       <c r="H16" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="I16" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="J16" t="s">
         <v>99</v>
@@ -4507,7 +5793,7 @@
     </row>
     <row r="17" spans="9:9" x14ac:dyDescent="0.3">
       <c r="I17" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se ha terminado de agregar mas del 80% de informacion
</commit_message>
<xml_diff>
--- a/Guia de arboles y otras plantas nativas de Mty.xlsx
+++ b/Guia de arboles y otras plantas nativas de Mty.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uanledu-my.sharepoint.com/personal/carlos_martinezhrn_uanl_edu_mx/Documents/Documents/Github Projects/Guia-de-Arboles-y-Plantas-Nativas-de-Monterrey/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="855" documentId="8_{2025911F-8D31-4388-B950-35610A59B777}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2AA1BBFD-8AD6-407B-83F6-B3ACDA6CEA6F}"/>
+  <xr:revisionPtr revIDLastSave="1174" documentId="8_{2025911F-8D31-4388-B950-35610A59B777}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7885D84E-ECB0-448B-B4DE-7D145EF6F6C8}"/>
   <bookViews>
-    <workbookView xWindow="9972" yWindow="36" windowWidth="13080" windowHeight="5148" firstSheet="8" activeTab="10" xr2:uid="{E5260BE0-913F-4F2E-A4BB-A577272EBBD7}"/>
+    <workbookView xWindow="9264" yWindow="72" windowWidth="13704" windowHeight="9168" firstSheet="11" activeTab="11" xr2:uid="{E5260BE0-913F-4F2E-A4BB-A577272EBBD7}"/>
   </bookViews>
   <sheets>
     <sheet name="Calendario de Floracion" sheetId="6" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="865" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1034" uniqueCount="353">
   <si>
     <t>Nombre Comun</t>
   </si>
@@ -692,9 +692,6 @@
     <t>Valle o Desierto</t>
   </si>
   <si>
-    <t>Codigo RGB</t>
-  </si>
-  <si>
     <t>Echinocactus y Ferocactus</t>
   </si>
   <si>
@@ -896,14 +893,310 @@
     <t>Cercis canadensis</t>
   </si>
   <si>
-    <t>Caesa</t>
+    <t>J</t>
+  </si>
+  <si>
+    <t>Todas las zonas del area metropolitana cuya topografia aes plana o de bajo relieve. Para utilidad de esta guia, seconsideran valles la totalidad de los municipios de Guadalupe, San Nicolas de los Garza, Benito Juarez y parte de Escobedo. Tambien se incluye el municipio de Monterrey, con excepcion de las faldas del cerro de la silla, la zona del Huajuco y la cara norte del cerro de las Mitras. En San Pedro se considero valle la zona baja del municipio, incluyendo Valle Oriente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El area de montaña se encuentra principalmente en los municipios de San Pedro Garza Garcia, Monterrey y Santiago. En el primero se consideran las faldas y las partes altas de la Sierra Madre Oriental, y los cerros de El Mirador y La Corona. Varias areas residenciales se encuentran en las cercanias del Parque Ecologico Chipinque, que es habitat de muchas de las especies listadas en esta guia. En Monterrey, el area de montaña se encuentra en las faldas del cerro de La Silla en la colonia Contry La Silla y en el Cañon del Huajuco. En el Municipio de Santiago se considera la cabecera municipal y sus alrededores, asi como la falda noeste de La Silla </t>
+  </si>
+  <si>
+    <t>La mayoria del municipio de Santa Catarina en su parte baja, asi como el extremo poniente del municipio de Escobedo y parte de Apodaca. En esta el tipo de suelo y el asoleamiento cambian, por lo que se recomiendan las especies mas resistentes a sequias, que pueden desarrollarse en suelos pobres</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Se recomienda el uso de las esoecies identificadas con este habitat en las orillas de lagos, naturales o artificiales, presas, arroyos y rios. En ocaciones se considera dentro de las especificaciones de este habitat a los principales escurrimientos pluviales naturales de la ciudad donde aun existe flujo intenso de agua durante las lluvias </t>
+  </si>
+  <si>
+    <t>Cualquier tipo de suelo que permita que el agua, ya sea de riego o pluvial, sea rapidamente absorbida y no genera saturacion en el area de la raiz. Generalmente estos suelos son pedregosos o archillosos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suelos con capacidad de saturarse por un tiempo. Permiten buena permeabilidad hacia la raiz del arbol sin llegar a saturarse facilmente. La mayoria de los arboles y plantas incluidas en esta guia se adapta con facilidad a este tipo de suelo </t>
+  </si>
+  <si>
+    <t>Suelos saturados, cenagosos, en los que el agua pluvial o de riego tiene una absorcion lenta, provocando que la raiz del arbol se mantenga por mas tiempo humeda. Usualmente estos suelos contienen mucha materia organica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Caesalpinia mexicana </t>
+  </si>
+  <si>
+    <t>Acacia farnesiana</t>
+  </si>
+  <si>
+    <t>Sapindus saponaria</t>
+  </si>
+  <si>
+    <t>Arbutus texana</t>
+  </si>
+  <si>
+    <t>Ericaceae</t>
+  </si>
+  <si>
+    <t>Prosopis glandulosa</t>
+  </si>
+  <si>
+    <t>Chilopsis linearis</t>
+  </si>
+  <si>
+    <t>Bignoniaceae</t>
+  </si>
+  <si>
+    <t>Ungnadia speciosa</t>
+  </si>
+  <si>
+    <t>Parkinsonia texana</t>
+  </si>
+  <si>
+    <t>Codigo HEX</t>
+  </si>
+  <si>
+    <t>RGB</t>
+  </si>
+  <si>
+    <t>102, 166, 87</t>
+  </si>
+  <si>
+    <t>Pinus cembrpides</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no </t>
+  </si>
+  <si>
+    <t>Retama</t>
+  </si>
+  <si>
+    <t>Parkinsonia aculeata</t>
+  </si>
+  <si>
+    <t>Drenado Medio o Drenado Lento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tronadora </t>
+  </si>
+  <si>
+    <t>Tecoma stans</t>
+  </si>
+  <si>
+    <t>151, 79, 47</t>
+  </si>
+  <si>
+    <t>#974F2F</t>
+  </si>
+  <si>
+    <t>#d99986</t>
+  </si>
+  <si>
+    <t>#9cd199</t>
+  </si>
+  <si>
+    <t>#66a657</t>
+  </si>
+  <si>
+    <t>217, 153, 134</t>
+  </si>
+  <si>
+    <t>156, 209, 153</t>
+  </si>
+  <si>
+    <t>100, 148, 107</t>
+  </si>
+  <si>
+    <t>139, 155, 69</t>
+  </si>
+  <si>
+    <t>215, 193, 125</t>
+  </si>
+  <si>
+    <t>47, 109, 56</t>
+  </si>
+  <si>
+    <t>110, 192, 99</t>
+  </si>
+  <si>
+    <t>158, 115, 72</t>
+  </si>
+  <si>
+    <t>114, 60, 53</t>
+  </si>
+  <si>
+    <t>203, 196, 116</t>
+  </si>
+  <si>
+    <t>68, 109, 55</t>
+  </si>
+  <si>
+    <t>151, 166, 64</t>
+  </si>
+  <si>
+    <t>64, 70, 44</t>
+  </si>
+  <si>
+    <t>188, 183, 98</t>
+  </si>
+  <si>
+    <t>126, 147, 77</t>
+  </si>
+  <si>
+    <t>165, 161, 129</t>
+  </si>
+  <si>
+    <t>205, 172, 132</t>
+  </si>
+  <si>
+    <t>129, 95, 62</t>
+  </si>
+  <si>
+    <t>#64946B</t>
+  </si>
+  <si>
+    <t>#8B9B45</t>
+  </si>
+  <si>
+    <t>#D7C17D</t>
+  </si>
+  <si>
+    <t>#CBC474</t>
+  </si>
+  <si>
+    <t>#2F6D38</t>
+  </si>
+  <si>
+    <t>E l sotol aporta un gran complemento al jardín árido, ya que posee un aspecto peculiar que se debate entre la rigidez de un agave y la soltura de un pasto. Sus pencas u hojas suelen ser semirrígidas, parten todas del mismo centro y trazan, en ocasiones, una media esfera casi perfecta. Esta forma se complementa con un espectacular quiote está cubierto totalmente de la florescencia. El sotol es muy adaptable a diversas condiciones climáticas y de suelos. Se encuentra en sitios de muy alta salinidad, siendo una especie dominante y presentando un perfil muy rígido. También puede soportar ambientes sutilmente más húmedos, en los que sus hojas llegan a vencerse para adquirir un aspecto más cercano a un pasto silvestre. El sotol, como casi todas las especies desérticas, presenta espinas a lo largo de sus hojas; éstas son muy continuas y pequeñas, asemejándose a una hoja serrada.</t>
+  </si>
+  <si>
+    <t>Una época de floración breve, entre marzo o abril, no es motivo para dejar de apreciar esta especie de cactus  que en plena florescencia da color al suelo árido. La pitaya es un ideal complemento del jardín desértico. Si
+bien su altura no rebasa los cuarenta centímetros, sus numerosas espinas de gran tamaño y su copiosa ramificación
+la hacen atractiva dentro de este tipo de jardines. Al conjunto principal de tallos en forma cilíndrica se le integran
+nuevos que crecen desde la parte baja, inicialmente en una
+dirección horizontal para luego enderezarse. Hay pitayas
+que pueden llegar a tener hasta cien tallos, lo que permite
+que su impacto en el paisaje sea mayor.
+Sus espinas llegan a medir tres o cuatro centímetros y suelen aportar un elemento estético al cactus, ya que con
+cierta iluminación del sol se tornan amarillas o doradas y transforman la apreciación cromática
+de la planta. El efecto se complementa con el color violeta o
+morado intenso de las flores, que
+se abren de día alcanzando los
+diez centímetros de diámetro</t>
+  </si>
+  <si>
+    <t>La identidad florística de México está representada por el ahuehuete como árbol, el nopal como cactus y, sin duda, la yuca como palma. Su presencia en el paisaje del desierto mexicano es majestuosa. La yuca posee un potencial paisajístico único, al desempeñar dos funciones: la de especie de carácter desértico y la de escultura natural. Su forma rígida y rústica, y sus cabezales siempre verdes y aleatorios en su crecimiento y dirección provocan que esta especie se convierta en un monumento en el contexto urbano. Existen varios proyectos de paisaje en los que se ha utilizado la yuca para reafirmar espacios, perspectivas o simplemente para marcar un punto focal. Parece por sí solo un elemento arquitectónico. Esta especie, al ser nativa del hábitat desértico, casi no requiere mantenimiento y, a pesar de que su crecimiento es lento, una vez desarrollada suele ser espectacular. Se puede plantar en estacionamientos, donde se deberá aumentar su densidad para proyectar una sombra útil. También se puede utilizar en jardines residenciales, plazas comerciales, camellones y hasta banquetas, donde será importante considerar el espacio para su follaje.</t>
+  </si>
+  <si>
+    <t>Otra especie de porte escultórico, el ocotillo, destaca por el profuso follaje adosado a sus ramas y por la exuberante floración roja que nace en el ápice de la planta. El ocotillo es un sobreviviente. Su presencia y majestuosidad se pueden apreciar tanto en desiertos fértiles como en sitios inhóspitos. Usualmente carente de hojas, basta una ligera lluvia o un riego menor para que sus ramas espinosas se cubran de un denso follaje verde brillante. Durante la primavera y parte del verano su flor roja resalta en los paisajes. A pesar de su belleza singular, la albarda tiene un uso restringido en el contexto urbano, debido principalmente a la presencia de sus espinas rígidas de gran tamaño que representan una amenaza para peatones. Considerando esto, se recomienda su uso como elemento visual y escultórico dentro de un área sin tránsito peatonal, pero donde se pueda apreciar su belleza. El ocotillo atrae gran cantidad de aves que todo el año utilizan sus ramas como sitios de descanso u observación. En tiempos de floración este efecto es más común</t>
+  </si>
+  <si>
+    <t>El ícono florístico más representativo de México, el nopal, omnipresente en la alimentación de los mexicanos, ahora se recomienda también como una especie con gran potencial estético. El nopal presenta una oportunidad magnífica para un jardín en el cual pueda realizar funciones estéticas y alimenticias. Por un lado, la abundancia y exuberancia de su flor amarilla, en ocasiones naranja, provoca un auténtico espectáculo primaveral; por otro, el fruto conocido como tuna y la misma penca son manjares de nuestra gastronomía. El intenso color que el nopal de monte posee durante la época de floración, entre abril y julio, permite que esta especie se convierta en el punto focal de un jardín residencial o, si se planta en conjunto, se puede utilizar en áreas más extendidas multiplicando el efecto cromático. Durante el resto del año el nopal se mantiene vigoroso y verde, atrayendo fauna en búsqueda de alimento o de cobijo. La aportación estética del nopal en un diseño de paisaje va más allá de la forma y el color, ya es símbolo de la mexicanidad. Del nopal es posible comer su fruto y sus pencas, es decir, casi la totalidad de la planta. Cuando se busca regenerar terrenos en el olvido, se pueden desarrollar cultivos urbanos de nopal permitiendo a la comunidad ser partícipe de la cosecha. El nopal de monte es resistente a las sequías y al frío intenso, incluso a las nevadas, por lo que se sugiere su uso en jardines o áreas verdes de muy bajo mantenimiento</t>
+  </si>
+  <si>
+    <t>Símbolo del desierto y de nuestra identidad natural, el maguey posee un porte que denota fuerza y resistencia, además de aportar belleza al paisaje. El atractivo de esta especie radica en sus implacables pencas de color azul verdoso, las cuales sólo llegan a doblegarse si han alcanzado una gran altura, en cuyo caso el maguey ya se habrá convertido en un patrimonio del lugar donde se encuentre. Al igual que todas las especies desérticas, el maguey sobrevive a las sequías y no requiere un mantenimiento mayor, sólo es necesario dotarlo del espacio necesario para desarrollarse en plenitud. Un maguey solitario puede representar un remate visual en jardines residenciales y, en algunos casos, comerciales. Se recomienda su uso masivo en camellones, donde es necesario evitar el cruce peatonal, y en jardineras bien delimitadas dentro de plazas o espacios públicos.</t>
+  </si>
+  <si>
+    <t>Una de las especies más comunes en el paisaje desértico de Nuevo León, la lechuguilla soporta el más extremo clima, ofreciendo una garantía de sobrevivencia única. Sus pencas de color amarillento y verde se distribuyen radialmente desde su centro, quedando las más viejas en el exterior y las jóvenes en el interior. Como agave, su resistencia a la sequía es alta; logra sobrevivir en condiciones de escasez. La lechuguilla es rígida y, debido a que sus pencas están aserradas, presenta un riesgo para el peatón, por lo que se recomienda plantar en espacios bien definidos. Su uso en jardines desérticos puede aportar follaje bajo, lo que genera una densidad que se aprecia exuberante. Esta especie se encuentra en el repertorio vegetal ideal para las azoteas verdes, espacios urbanos que usualmente son afectados por condiciones similares al desierto, tales como sol permanente, fuertes vientos y pérdida de suelo.</t>
+  </si>
+  <si>
+    <t>L a gobernadora, omnipresente en el desierto chihuahuense en cuyo extremo oriente se encuentra Monterrey, domina el paisaje y lo perfuma con el intenso aroma de sus flores. La gobernadora es el arbusto del desierto. Por lo general rodeado de cactáceas, agaves, yucas y ocotillos, esta especie se destaca por su forma densamente ramificada desde el piso y sus hojas de tonos verde oscuros. Durante su floración, de marzo a septiembre, se tiñe de un tono amarillento que le otorga un nuevo valor paisajístico. Se recomienda su uso en jardines como complemento de un ambiente desértico, o mezclada con especies no áridas, ya que su apariencia de arbusto le permite crear relaciones estéticas con otros setos. La gobernadora es altamente resistente a la sequía y al frío, por lo que su mantenimiento es mínimo, lo que impulsa su uso en jardines sustentables donde resulta esencial el ahorro de energía y recursos hídricos. Antes de desmontar un área, en la que se encuentre la gobernadora, se recomienda conservarla en su ubicación original para evitar trasplantes.</t>
+  </si>
+  <si>
+    <t>Tal como otras especies desérticas, la biznaga es característica del paisaje árido. Muestra cierta agresividad estética, debido a sus numerosas espinas que a la vez le otorgan belleza única. De forma esférica cuando joven, que se convierte en una especie de cilindro al madurar, esta especie posee evidentes muestras de la sabiduría natural del desierto. Las nervaduras o surcos que recorren su circunferencia captan y dirigen la escasa agua que obtienen a sus raíces evitando pérdidas, hasta finalmente almacenarla en el mismo cuerpo de la biznaga, dándole esa forma tan atractiva. Su presencia en un jardín árido es esencial, ya que contrasta con el efecto provocado por agaves como lechuguillas y magueyes. Su floración en la cresta de la planta llama mucho la atención.</t>
+  </si>
+  <si>
+    <t>Al igual que la lantana, la veintiunilla o asclepia es una favorita de las mariposas, especialmente las monarcas cuya presencia en el otoño es más evidente alrededor de esta planta. A la distancia, la flor de la asclepia es similar en color y
+tamaño a la de la lantana; sin embargo, son especies muy
+distintas, las hojas de la veintiunilla son alargadas y más
+ordenadas o regulares, lo que redunda en una apariencia
+más agradable durante el invierno.
+Su uso en un jardín pequeño puede ser de forma individual
+o combinado con rastreras o arbustos con flor, creando
+espacios multicolores muy llamativos que sirven para resaltar algún elemento, o simplemente como remate visual
+desde alguna habitación. La veintiunilla se debe considerar
+como un arbusto bajo, más que como una rastrera, por
+lo que su uso en grupos como setos de división es muy
+aprovechable.</t>
+  </si>
+  <si>
+    <t>El complemento de cualquier proyecto de paisaje o área verde en general es el pasto. La cubierta que éste genera permite asumir el espacio como un sitio agradable y acogedor. Existe una gran variedad de pastos nativos en nuestra región, crecen sin necesidad de cuidados y poca agua. De hecho, varios de ellos sobreviven en condiciones de sequía intensa, requiriendo no más de veinte milímetros de lluvia al año –Monterrey recibe entre 300 y 600 milímetros. Estos pastos ya se encuentran en el paisaje urbano, principalmente en terrenos o áreas que han sido intervenidas por el hombre, ya sea por desmonte o por movimientos de tierra. La mayoría de los pastos nativos crecen hasta los sesenta centímetros, por lo que en su estado natural son atractivos y pueden mantenerse como tal en proyectos donde su función sea más visual que de uso intensivo. Su floración es mayor si no se intervienen, lo que crea un efecto paisajístico muy atractivo cuando el viento mueve los ligeros tallos que soportan las flores. Cuando el uso del pasto va a ser como superficie de juego o peatonal, se puede podar, logrando un efecto similar al de un pasto tradicional. El máximo requisito de estas especies es obtener luz directa del sol durante todo el día, por lo que no se recomiendan para zonas sombreadas.</t>
+  </si>
+  <si>
+    <t>E s una hierba silvestre poseedora de una flor color azul profundo que, si se planta masivamente, durante la primavera se convierte en una cama cromática del paisaje urbano. El lupino es muy utilizado en Texas a la orilla de las autopistas y ofrece a los conductores otra perspectiva de lo
+que puede ser un viaje en carretera. Durante la primavera
+estos caminos se tiñen de azul intenso a lo largo de cientos de kilómetros y, durante el resto del año, los suelos
+se observan verdes y siempre cubiertos de vegetación.
+En Nuevo León se podría lograr un efecto similar si utilizáramos más ésta y otras especies de hierbas o flores
+silvestres. A simple vista el lupino es una planta siempre
+verde cuya altura no rebasa los cincuenta centímetros.
+Puede cubrir rápidamente el suelo dotándolo de vida en
+situaciones de clima adverso, ya que los requerimientos de
+agua del lupino son mínimos.
+Se recomienda en áreas de sol intenso y si
+se planta en un suelo por primera vez
+es benéfico porque inyecta nitrógeno
+a la tierra, permitiendo un mejor
+enraizamiento del lupino.</t>
+  </si>
+  <si>
+    <t>L a belleza de las mariposas despierta una gran admiración y, para deleitarse con la presencia de estos insectos, es necesario atraerlos y nada mejor que la lantana para lograrlo. Esta especie, identificada como Lantana urticoides u horrida
+por Hayek es un auténtico manjar para diversas especies de
+insectos y aves, a los que atrae nueve meses del año. El color
+de sus flores varía en tonos cálidos. La lantana es una subarbustiva que en ocasiones crece hasta el tamaño de arbusto.
+La lantana tiene un alto potencial paisajístico. Su resistencia
+a las altas temperaturas y el relativo bajo mantenimiento
+que requiere –aún cuando aprecia mucho un riego constante– la hacen ideal para ambientar grandes extensiones de
+áreas verdes, creando alfombras cromáticas que a su vez
+están siempre llenas de vida. También es posible establecerla en detalles más puntuales, aunque en lo individual es
+muy irregular y poco atractiva en invierno.
+A pesar de ser una especie gustosa del sol intenso, se le
+puede encontrar en ambientes boscosos y sombreados,
+aunque su floración es menos intensa.</t>
+  </si>
+  <si>
+    <t>Como muchas de las especies adaptadas al matorral submontano, la belleza, frangancia y detalle del guajillo se aprecian mejor en forma de arbusto Posee características estéticas que le confieren un potencial paisajístico amplio; en ocasiones puede integrarse a un
+jardín de condiciones áridas y, en otras, sus hojas similares
+al helecho logran que parezca una especie más relacionada con ambientes húmedos.
+El atractivo mayor del guajillo es su profusa floración,
+que provee alimento para un gran número de mariposas
+e insectos. Cualquier acercamiento a la copa de este gran
+arbusto permite escuchar y observar una vida intensa.
+Como especie paisajística, el guajillo puede utilizarse
+en jardines residenciales de escala grande, donde pueda
+aprovecharse su copa baja o, también, como especie regeneradora de terrenos en abandono, pues impulsa el crecimiento de otras especies mayores.</t>
+  </si>
+  <si>
+    <t>E n ocasiones descrita como especie tropical, la dodónea se presenta en Nuevo León como un arbusto de gran atractivo paisajístico capaz de resistir las condiciones climáticas de la región. La característica principal de esta especie es su inusual resistencia a la sequía. Esto se debe a la capa resinosa de sus
+hojas que evita la pérdida de agua. Debido a ello la dodónea
+es un excelente arbusto con gran potencial en el paisaje
+urbano. Su follaje es siempre verde y el tono de sus hojas
+se aprecia joven, brillante.
+Por la forma de su copa, irregular y extendida a lo ancho,
+y por el hecho de presentar varios troncos, esta especie
+puede sobresalir de manera individual, aunque cuando se
+planta en grupos el efecto de barrera o de pantalla se hace
+más evidente. Su uso es recomendado en espacios públicos
+donde se requiera ambientar las áreas entre árboles, creando una atmósfera más boscosa, más densa.
+Su crecimiento es ágil y su resistencia a la falta de mantenimiento es alta, por lo que su uso como regeneradora de
+espacios verdes o fijadora de suelos es aconsejable.</t>
+  </si>
+  <si>
+    <t>E l arbusto por excelencia de Nuevo León, el cenizo, es conocido en Texas como el “arbusto barómetro” debido a que su sorprendente floración depende de la humedad en el ambiente y de la precipitación pluvial Un magnífico espectáculo es ver cubrirse las faldas de
+las montañas o cerros que rodean Monterrey de una sutil
+pantalla violeta, producida por la intensa floración del
+cenizo. Su abundancia en el matorral permite que éste
+se tiña de color cada vez que se presentan o están por
+suceder lluvias.
+Su sensibilidad a la lluvia y su capacidad para sobrellevar
+la ausencia de ésta permiten que el cenizo sea utilizado
+como especie de bajo mantenimiento, a la vez que de
+él se obtienen beneficios estéticos en un jardín de alto
+cuidado.
+El cenizo es ideal para barreras entre propiedades, o para
+isletas de estacionamientos. Su uso se recomienda en
+grupos, para exagerar su efecto. Su forma es irregular</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -911,8 +1204,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -973,6 +1272,60 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF66A657"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9CD199"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF974F2F"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD99986"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF64946B"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF8B9B45"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCBC474"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD7C17D"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF2F6D38"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -986,7 +1339,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1000,9 +1353,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1026,10 +1389,16 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF2F6D38"/>
+      <color rgb="FFCBC474"/>
+      <color rgb="FFD7C17D"/>
+      <color rgb="FF8B9B45"/>
+      <color rgb="FF64946B"/>
+      <color rgb="FF974F2F"/>
+      <color rgb="FFD99986"/>
+      <color rgb="FF9CD199"/>
+      <color rgb="FF66A657"/>
       <color rgb="FF7F4949"/>
-      <color rgb="FFC96565"/>
-      <color rgb="FFB77F7B"/>
-      <color rgb="FFD5C887"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1379,7 +1748,7 @@
   <dimension ref="A1:AA56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Z47" sqref="Z47"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1400,54 +1769,54 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11" t="s">
+      <c r="E1" s="18"/>
+      <c r="F1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11" t="s">
+      <c r="G1" s="18"/>
+      <c r="H1" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11" t="s">
+      <c r="I1" s="18"/>
+      <c r="J1" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11" t="s">
+      <c r="K1" s="18"/>
+      <c r="L1" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11" t="s">
+      <c r="M1" s="18"/>
+      <c r="N1" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11" t="s">
+      <c r="O1" s="18"/>
+      <c r="P1" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="11" t="s">
+      <c r="Q1" s="18"/>
+      <c r="R1" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="S1" s="11"/>
-      <c r="T1" s="11" t="s">
+      <c r="S1" s="18"/>
+      <c r="T1" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="U1" s="11"/>
-      <c r="V1" s="11" t="s">
+      <c r="U1" s="18"/>
+      <c r="V1" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="W1" s="11"/>
-      <c r="X1" s="11" t="s">
+      <c r="W1" s="18"/>
+      <c r="X1" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="Y1" s="11"/>
-      <c r="Z1" s="11" t="s">
+      <c r="Y1" s="18"/>
+      <c r="Z1" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="AA1" s="11"/>
+      <c r="AA1" s="18"/>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2">
@@ -2313,9 +2682,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.33203125" customWidth="1"/>
     <col min="2" max="2" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.21875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.44140625" bestFit="1" customWidth="1"/>
@@ -2402,10 +2771,10 @@
         <v>108</v>
       </c>
       <c r="C2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E2" t="s">
         <v>158</v>
@@ -2452,7 +2821,7 @@
         <v>109</v>
       </c>
       <c r="C3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D3" t="s">
         <v>207</v>
@@ -2473,7 +2842,7 @@
         <v>200</v>
       </c>
       <c r="J3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="K3" t="s">
         <v>196</v>
@@ -2491,7 +2860,7 @@
         <v>8</v>
       </c>
       <c r="P3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
@@ -2502,7 +2871,7 @@
         <v>110</v>
       </c>
       <c r="C4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D4" t="s">
         <v>182</v>
@@ -2541,7 +2910,7 @@
         <v>10</v>
       </c>
       <c r="P4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.3">
@@ -2552,7 +2921,7 @@
         <v>111</v>
       </c>
       <c r="C5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D5" t="s">
         <v>182</v>
@@ -2591,7 +2960,7 @@
         <v>12</v>
       </c>
       <c r="P5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.3">
@@ -2602,7 +2971,7 @@
         <v>112</v>
       </c>
       <c r="C6" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D6" t="s">
         <v>182</v>
@@ -2641,7 +3010,7 @@
         <v>8</v>
       </c>
       <c r="P6" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.3">
@@ -2652,7 +3021,7 @@
         <v>113</v>
       </c>
       <c r="C7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D7" t="s">
         <v>182</v>
@@ -2691,7 +3060,7 @@
         <v>9</v>
       </c>
       <c r="P7" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.3">
@@ -2702,10 +3071,10 @@
         <v>114</v>
       </c>
       <c r="C8" t="s">
+        <v>253</v>
+      </c>
+      <c r="D8" t="s">
         <v>254</v>
-      </c>
-      <c r="D8" t="s">
-        <v>255</v>
       </c>
       <c r="E8" t="s">
         <v>158</v>
@@ -2741,7 +3110,7 @@
         <v>8</v>
       </c>
       <c r="P8" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.3">
@@ -2752,10 +3121,10 @@
         <v>115</v>
       </c>
       <c r="C9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D9" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E9" t="s">
         <v>160</v>
@@ -2856,7 +3225,7 @@
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="I13" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
   </sheetData>
@@ -2868,20 +3237,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E60A5AA-C027-4451-B966-CFECF96F6C4B}">
   <dimension ref="A1:U24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.21875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.21875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.88671875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.88671875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="6.33203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="4" bestFit="1" customWidth="1"/>
@@ -2963,10 +3334,10 @@
         <v>138</v>
       </c>
       <c r="C2" t="s">
+        <v>241</v>
+      </c>
+      <c r="D2" t="s">
         <v>242</v>
-      </c>
-      <c r="D2" t="s">
-        <v>243</v>
       </c>
       <c r="E2" t="s">
         <v>158</v>
@@ -2981,7 +3352,7 @@
         <v>163</v>
       </c>
       <c r="I2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="J2" t="s">
         <v>98</v>
@@ -3013,7 +3384,7 @@
         <v>139</v>
       </c>
       <c r="C3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D3" t="s">
         <v>207</v>
@@ -3031,7 +3402,7 @@
         <v>160</v>
       </c>
       <c r="I3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="J3" t="s">
         <v>97</v>
@@ -3063,10 +3434,10 @@
         <v>140</v>
       </c>
       <c r="C4" t="s">
+        <v>268</v>
+      </c>
+      <c r="D4" t="s">
         <v>269</v>
-      </c>
-      <c r="D4" t="s">
-        <v>270</v>
       </c>
       <c r="E4" t="s">
         <v>160</v>
@@ -3084,7 +3455,7 @@
         <v>189</v>
       </c>
       <c r="J4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="K4" t="s">
         <v>196</v>
@@ -3113,10 +3484,10 @@
         <v>141</v>
       </c>
       <c r="C5" t="s">
+        <v>271</v>
+      </c>
+      <c r="D5" t="s">
         <v>272</v>
-      </c>
-      <c r="D5" t="s">
-        <v>273</v>
       </c>
       <c r="E5" t="s">
         <v>158</v>
@@ -3134,7 +3505,7 @@
         <v>189</v>
       </c>
       <c r="J5" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="K5" t="s">
         <v>175</v>
@@ -3163,7 +3534,7 @@
         <v>142</v>
       </c>
       <c r="C6" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D6" t="s">
         <v>207</v>
@@ -3184,7 +3555,7 @@
         <v>189</v>
       </c>
       <c r="J6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="K6" t="s">
         <v>176</v>
@@ -3213,10 +3584,10 @@
         <v>143</v>
       </c>
       <c r="C7" t="s">
+        <v>276</v>
+      </c>
+      <c r="D7" t="s">
         <v>277</v>
-      </c>
-      <c r="D7" t="s">
-        <v>278</v>
       </c>
       <c r="E7" t="s">
         <v>160</v>
@@ -3234,7 +3605,7 @@
         <v>189</v>
       </c>
       <c r="J7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="K7" t="s">
         <v>175</v>
@@ -3263,10 +3634,10 @@
         <v>144</v>
       </c>
       <c r="C8" t="s">
+        <v>278</v>
+      </c>
+      <c r="D8" t="s">
         <v>279</v>
-      </c>
-      <c r="D8" t="s">
-        <v>280</v>
       </c>
       <c r="E8" t="s">
         <v>160</v>
@@ -3284,7 +3655,7 @@
         <v>189</v>
       </c>
       <c r="J8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="K8" t="s">
         <v>175</v>
@@ -3313,7 +3684,7 @@
         <v>145</v>
       </c>
       <c r="C9" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D9" t="s">
         <v>207</v>
@@ -3334,7 +3705,7 @@
         <v>189</v>
       </c>
       <c r="J9" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="K9" t="s">
         <v>181</v>
@@ -3363,10 +3734,46 @@
         <v>146</v>
       </c>
       <c r="C10" t="s">
-        <v>282</v>
+        <v>289</v>
       </c>
       <c r="D10" t="s">
         <v>207</v>
+      </c>
+      <c r="E10" t="s">
+        <v>160</v>
+      </c>
+      <c r="F10" t="s">
+        <v>83</v>
+      </c>
+      <c r="G10" t="s">
+        <v>86</v>
+      </c>
+      <c r="H10" t="s">
+        <v>163</v>
+      </c>
+      <c r="I10" t="s">
+        <v>189</v>
+      </c>
+      <c r="J10" t="s">
+        <v>98</v>
+      </c>
+      <c r="K10" t="s">
+        <v>196</v>
+      </c>
+      <c r="L10" t="s">
+        <v>181</v>
+      </c>
+      <c r="M10">
+        <v>5.5</v>
+      </c>
+      <c r="N10">
+        <v>4</v>
+      </c>
+      <c r="O10">
+        <v>5</v>
+      </c>
+      <c r="P10" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.3">
@@ -3376,8 +3783,47 @@
       <c r="B11" t="s">
         <v>147</v>
       </c>
+      <c r="C11" t="s">
+        <v>290</v>
+      </c>
       <c r="D11" t="s">
         <v>207</v>
+      </c>
+      <c r="E11" t="s">
+        <v>158</v>
+      </c>
+      <c r="F11" t="s">
+        <v>82</v>
+      </c>
+      <c r="G11" t="s">
+        <v>86</v>
+      </c>
+      <c r="H11" t="s">
+        <v>160</v>
+      </c>
+      <c r="I11" t="s">
+        <v>244</v>
+      </c>
+      <c r="J11" t="s">
+        <v>184</v>
+      </c>
+      <c r="K11" t="s">
+        <v>175</v>
+      </c>
+      <c r="L11" t="s">
+        <v>175</v>
+      </c>
+      <c r="M11">
+        <v>5</v>
+      </c>
+      <c r="N11">
+        <v>5</v>
+      </c>
+      <c r="O11">
+        <v>6</v>
+      </c>
+      <c r="P11" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.3">
@@ -3387,6 +3833,48 @@
       <c r="B12" t="s">
         <v>148</v>
       </c>
+      <c r="C12" t="s">
+        <v>291</v>
+      </c>
+      <c r="D12" t="s">
+        <v>199</v>
+      </c>
+      <c r="E12" t="s">
+        <v>160</v>
+      </c>
+      <c r="F12" t="s">
+        <v>82</v>
+      </c>
+      <c r="G12" t="s">
+        <v>85</v>
+      </c>
+      <c r="H12" t="s">
+        <v>163</v>
+      </c>
+      <c r="I12" t="s">
+        <v>189</v>
+      </c>
+      <c r="J12" t="s">
+        <v>97</v>
+      </c>
+      <c r="K12" t="s">
+        <v>181</v>
+      </c>
+      <c r="L12" t="s">
+        <v>181</v>
+      </c>
+      <c r="M12">
+        <v>6</v>
+      </c>
+      <c r="N12">
+        <v>5</v>
+      </c>
+      <c r="O12">
+        <v>6.5</v>
+      </c>
+      <c r="P12" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13">
@@ -3395,6 +3883,48 @@
       <c r="B13" t="s">
         <v>149</v>
       </c>
+      <c r="C13" t="s">
+        <v>292</v>
+      </c>
+      <c r="D13" t="s">
+        <v>293</v>
+      </c>
+      <c r="E13" t="s">
+        <v>158</v>
+      </c>
+      <c r="F13" t="s">
+        <v>82</v>
+      </c>
+      <c r="G13" t="s">
+        <v>87</v>
+      </c>
+      <c r="H13" t="s">
+        <v>183</v>
+      </c>
+      <c r="I13" t="s">
+        <v>189</v>
+      </c>
+      <c r="J13" t="s">
+        <v>97</v>
+      </c>
+      <c r="K13" t="s">
+        <v>196</v>
+      </c>
+      <c r="L13" t="s">
+        <v>181</v>
+      </c>
+      <c r="M13">
+        <v>5</v>
+      </c>
+      <c r="N13">
+        <v>2.5</v>
+      </c>
+      <c r="O13">
+        <v>4</v>
+      </c>
+      <c r="P13" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14">
@@ -3403,8 +3933,47 @@
       <c r="B14" t="s">
         <v>150</v>
       </c>
+      <c r="C14" t="s">
+        <v>294</v>
+      </c>
       <c r="D14" t="s">
         <v>207</v>
+      </c>
+      <c r="E14" t="s">
+        <v>160</v>
+      </c>
+      <c r="F14" t="s">
+        <v>81</v>
+      </c>
+      <c r="G14" t="s">
+        <v>86</v>
+      </c>
+      <c r="H14" t="s">
+        <v>160</v>
+      </c>
+      <c r="I14" t="s">
+        <v>244</v>
+      </c>
+      <c r="J14" t="s">
+        <v>99</v>
+      </c>
+      <c r="K14" t="s">
+        <v>196</v>
+      </c>
+      <c r="L14" t="s">
+        <v>196</v>
+      </c>
+      <c r="M14">
+        <v>6</v>
+      </c>
+      <c r="N14">
+        <v>7</v>
+      </c>
+      <c r="O14">
+        <v>7</v>
+      </c>
+      <c r="P14" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.3">
@@ -3414,6 +3983,48 @@
       <c r="B15" t="s">
         <v>151</v>
       </c>
+      <c r="C15" t="s">
+        <v>295</v>
+      </c>
+      <c r="D15" t="s">
+        <v>296</v>
+      </c>
+      <c r="E15" t="s">
+        <v>158</v>
+      </c>
+      <c r="F15" t="s">
+        <v>83</v>
+      </c>
+      <c r="G15" t="s">
+        <v>85</v>
+      </c>
+      <c r="H15" t="s">
+        <v>163</v>
+      </c>
+      <c r="I15" t="s">
+        <v>244</v>
+      </c>
+      <c r="J15" t="s">
+        <v>97</v>
+      </c>
+      <c r="K15" t="s">
+        <v>196</v>
+      </c>
+      <c r="L15" t="s">
+        <v>181</v>
+      </c>
+      <c r="M15">
+        <v>6</v>
+      </c>
+      <c r="N15">
+        <v>5</v>
+      </c>
+      <c r="O15">
+        <v>6</v>
+      </c>
+      <c r="P15" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16">
@@ -3422,43 +4033,250 @@
       <c r="B16" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C16" t="s">
+        <v>297</v>
+      </c>
+      <c r="D16" t="s">
+        <v>199</v>
+      </c>
+      <c r="E16" t="s">
+        <v>158</v>
+      </c>
+      <c r="F16" t="s">
+        <v>82</v>
+      </c>
+      <c r="G16" t="s">
+        <v>85</v>
+      </c>
+      <c r="H16" t="s">
+        <v>163</v>
+      </c>
+      <c r="I16" t="s">
+        <v>189</v>
+      </c>
+      <c r="J16" t="s">
+        <v>97</v>
+      </c>
+      <c r="K16" t="s">
+        <v>196</v>
+      </c>
+      <c r="L16" t="s">
+        <v>196</v>
+      </c>
+      <c r="M16">
+        <v>4.5</v>
+      </c>
+      <c r="N16">
+        <v>4</v>
+      </c>
+      <c r="O16">
+        <v>5</v>
+      </c>
+      <c r="P16" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
+        <v>298</v>
+      </c>
+      <c r="D17" t="s">
+        <v>207</v>
+      </c>
+      <c r="E17" t="s">
+        <v>158</v>
+      </c>
+      <c r="F17" t="s">
+        <v>83</v>
+      </c>
+      <c r="G17" t="s">
+        <v>86</v>
+      </c>
+      <c r="H17" t="s">
+        <v>163</v>
+      </c>
+      <c r="I17" t="s">
+        <v>244</v>
+      </c>
+      <c r="J17" t="s">
+        <v>98</v>
+      </c>
+      <c r="K17" t="s">
+        <v>196</v>
+      </c>
+      <c r="L17" t="s">
+        <v>181</v>
+      </c>
+      <c r="M17">
+        <v>5.5</v>
+      </c>
+      <c r="N17">
+        <v>4.5</v>
+      </c>
+      <c r="O17">
+        <v>6</v>
+      </c>
+      <c r="P17" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C18" t="s">
+        <v>302</v>
+      </c>
+      <c r="D18" t="s">
+        <v>262</v>
+      </c>
+      <c r="E18" t="s">
+        <v>158</v>
+      </c>
+      <c r="F18" t="s">
+        <v>83</v>
+      </c>
+      <c r="G18" t="s">
+        <v>87</v>
+      </c>
+      <c r="H18" t="s">
+        <v>183</v>
+      </c>
+      <c r="I18" t="s">
+        <v>189</v>
+      </c>
+      <c r="J18" t="s">
+        <v>98</v>
+      </c>
+      <c r="K18" t="s">
+        <v>303</v>
+      </c>
+      <c r="L18" t="s">
+        <v>181</v>
+      </c>
+      <c r="M18">
+        <v>6</v>
+      </c>
+      <c r="N18">
+        <v>4.5</v>
+      </c>
+      <c r="O18">
+        <v>4.5</v>
+      </c>
+      <c r="P18" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>47</v>
+        <v>304</v>
+      </c>
+      <c r="C19" t="s">
+        <v>305</v>
       </c>
       <c r="D19" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E19" t="s">
+        <v>158</v>
+      </c>
+      <c r="F19" t="s">
+        <v>83</v>
+      </c>
+      <c r="G19" t="s">
+        <v>86</v>
+      </c>
+      <c r="H19" t="s">
+        <v>163</v>
+      </c>
+      <c r="I19" t="s">
+        <v>244</v>
+      </c>
+      <c r="J19" t="s">
+        <v>306</v>
+      </c>
+      <c r="K19" t="s">
+        <v>196</v>
+      </c>
+      <c r="L19" t="s">
+        <v>181</v>
+      </c>
+      <c r="M19">
+        <v>6</v>
+      </c>
+      <c r="N19">
+        <v>6</v>
+      </c>
+      <c r="O19">
+        <v>7</v>
+      </c>
+      <c r="P19" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+        <v>307</v>
+      </c>
+      <c r="C20" t="s">
+        <v>308</v>
+      </c>
+      <c r="D20" t="s">
+        <v>296</v>
+      </c>
+      <c r="E20" t="s">
+        <v>160</v>
+      </c>
+      <c r="F20" t="s">
+        <v>82</v>
+      </c>
+      <c r="G20" t="s">
+        <v>87</v>
+      </c>
+      <c r="H20" t="s">
+        <v>163</v>
+      </c>
+      <c r="I20" t="s">
+        <v>189</v>
+      </c>
+      <c r="J20" t="s">
+        <v>98</v>
+      </c>
+      <c r="K20" t="s">
+        <v>181</v>
+      </c>
+      <c r="L20" t="s">
+        <v>181</v>
+      </c>
+      <c r="M20">
+        <v>4.5</v>
+      </c>
+      <c r="N20">
+        <v>3</v>
+      </c>
+      <c r="O20">
+        <v>4</v>
+      </c>
+      <c r="P20" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="E21" t="s">
         <v>158</v>
       </c>
@@ -3478,7 +4296,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="E22" t="s">
         <v>160</v>
       </c>
@@ -3498,7 +4316,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="E23" t="s">
         <v>159</v>
       </c>
@@ -3518,9 +4336,9 @@
         <v>99</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="I24" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
   </sheetData>
@@ -3532,13 +4350,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A920792F-CF3F-457F-833D-61DB879F4FB7}">
   <dimension ref="A1:U12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.33203125" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.6640625" customWidth="1"/>
+    <col min="10" max="10" width="17.88671875" customWidth="1"/>
+    <col min="11" max="11" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.33203125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="4" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="6" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="10" bestFit="1" customWidth="1"/>
@@ -3658,6 +4485,9 @@
       <c r="P2" t="s">
         <v>197</v>
       </c>
+      <c r="Q2" s="21" t="s">
+        <v>352</v>
+      </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3">
@@ -3708,6 +4538,9 @@
       <c r="P3" t="s">
         <v>197</v>
       </c>
+      <c r="Q3" s="21" t="s">
+        <v>351</v>
+      </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4">
@@ -3758,6 +4591,9 @@
       <c r="P4" t="s">
         <v>197</v>
       </c>
+      <c r="Q4" s="21" t="s">
+        <v>350</v>
+      </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5">
@@ -3808,6 +4644,9 @@
       <c r="P5" t="s">
         <v>205</v>
       </c>
+      <c r="Q5" s="21" t="s">
+        <v>349</v>
+      </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6">
@@ -3852,8 +4691,14 @@
       <c r="N6">
         <v>0.3</v>
       </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
       <c r="P6" t="s">
         <v>205</v>
+      </c>
+      <c r="Q6" s="21" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.3">
@@ -3893,8 +4738,20 @@
       <c r="L7" t="s">
         <v>181</v>
       </c>
+      <c r="M7">
+        <v>0.3</v>
+      </c>
+      <c r="N7">
+        <v>0.6</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
       <c r="P7" t="s">
         <v>205</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>347</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.3">
@@ -3945,6 +4802,9 @@
       </c>
       <c r="P8" t="s">
         <v>197</v>
+      </c>
+      <c r="Q8" s="21" t="s">
+        <v>346</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.3">
@@ -4021,7 +4881,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A892B183-95B1-429D-A4A3-E6ADC63D4933}">
   <dimension ref="A1:U14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -4116,10 +4978,10 @@
         <v>123</v>
       </c>
       <c r="C2" t="s">
+        <v>214</v>
+      </c>
+      <c r="D2" t="s">
         <v>215</v>
-      </c>
-      <c r="D2" t="s">
-        <v>216</v>
       </c>
       <c r="E2" t="s">
         <v>77</v>
@@ -4134,7 +4996,7 @@
         <v>89</v>
       </c>
       <c r="I2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J2" t="s">
         <v>97</v>
@@ -4156,6 +5018,9 @@
       </c>
       <c r="P2" t="s">
         <v>178</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>345</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
@@ -4166,10 +5031,10 @@
         <v>124</v>
       </c>
       <c r="C3" t="s">
+        <v>217</v>
+      </c>
+      <c r="D3" t="s">
         <v>218</v>
-      </c>
-      <c r="D3" t="s">
-        <v>219</v>
       </c>
       <c r="E3" t="s">
         <v>77</v>
@@ -4184,7 +5049,7 @@
         <v>78</v>
       </c>
       <c r="I3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J3" t="s">
         <v>97</v>
@@ -4206,6 +5071,9 @@
       </c>
       <c r="P3" t="s">
         <v>197</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>344</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
@@ -4216,10 +5084,10 @@
         <v>125</v>
       </c>
       <c r="C4" t="s">
+        <v>219</v>
+      </c>
+      <c r="D4" t="s">
         <v>220</v>
-      </c>
-      <c r="D4" t="s">
-        <v>221</v>
       </c>
       <c r="E4" t="s">
         <v>77</v>
@@ -4234,7 +5102,7 @@
         <v>78</v>
       </c>
       <c r="I4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J4" t="s">
         <v>97</v>
@@ -4256,6 +5124,9 @@
       </c>
       <c r="P4" t="s">
         <v>197</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>343</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.3">
@@ -4266,10 +5137,10 @@
         <v>126</v>
       </c>
       <c r="C5" t="s">
+        <v>221</v>
+      </c>
+      <c r="D5" t="s">
         <v>222</v>
-      </c>
-      <c r="D5" t="s">
-        <v>223</v>
       </c>
       <c r="E5" t="s">
         <v>77</v>
@@ -4284,7 +5155,7 @@
         <v>90</v>
       </c>
       <c r="I5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J5" t="s">
         <v>97</v>
@@ -4306,6 +5177,9 @@
       </c>
       <c r="P5" t="s">
         <v>197</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.3">
@@ -4316,10 +5190,10 @@
         <v>127</v>
       </c>
       <c r="C6" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E6" t="s">
         <v>77</v>
@@ -4334,7 +5208,7 @@
         <v>90</v>
       </c>
       <c r="I6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J6" t="s">
         <v>97</v>
@@ -4356,6 +5230,9 @@
       </c>
       <c r="P6" t="s">
         <v>197</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.3">
@@ -4363,13 +5240,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>233</v>
+      </c>
+      <c r="C7" t="s">
         <v>234</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>235</v>
-      </c>
-      <c r="D7" t="s">
-        <v>236</v>
       </c>
       <c r="E7" t="s">
         <v>77</v>
@@ -4384,7 +5261,7 @@
         <v>78</v>
       </c>
       <c r="I7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J7" t="s">
         <v>97</v>
@@ -4406,6 +5283,9 @@
       </c>
       <c r="P7" t="s">
         <v>197</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>340</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.3">
@@ -4416,10 +5296,10 @@
         <v>128</v>
       </c>
       <c r="C8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E8" t="s">
         <v>77</v>
@@ -4434,7 +5314,7 @@
         <v>89</v>
       </c>
       <c r="I8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J8" t="s">
         <v>97</v>
@@ -4455,7 +5335,10 @@
         <v>4</v>
       </c>
       <c r="P8" t="s">
-        <v>238</v>
+        <v>237</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>339</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.3">
@@ -4466,10 +5349,10 @@
         <v>129</v>
       </c>
       <c r="C9" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E9" t="s">
         <v>77</v>
@@ -4484,7 +5367,7 @@
         <v>78</v>
       </c>
       <c r="I9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J9" t="s">
         <v>97</v>
@@ -4506,6 +5389,9 @@
       </c>
       <c r="P9" t="s">
         <v>197</v>
+      </c>
+      <c r="Q9" s="21" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.3">
@@ -4516,10 +5402,10 @@
         <v>130</v>
       </c>
       <c r="C10" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D10" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E10" t="s">
         <v>77</v>
@@ -4534,7 +5420,7 @@
         <v>90</v>
       </c>
       <c r="I10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J10" t="s">
         <v>97</v>
@@ -4556,6 +5442,9 @@
       </c>
       <c r="P10" t="s">
         <v>197</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>337</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.3">
@@ -4790,7 +5679,7 @@
         <v>85</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="72" x14ac:dyDescent="0.3">
@@ -4801,7 +5690,7 @@
         <v>86</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
@@ -4812,7 +5701,7 @@
         <v>161</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
   </sheetData>
@@ -4854,7 +5743,7 @@
         <v>162</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
@@ -4865,7 +5754,7 @@
         <v>160</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
@@ -4876,7 +5765,7 @@
         <v>163</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
   </sheetData>
@@ -4886,19 +5775,20 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC4D8FC3-1EA8-4629-86A7-28B322CE7D58}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:O14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="78.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>155</v>
       </c>
@@ -4909,36 +5799,53 @@
         <v>157</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" ht="72" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C2" s="10" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C3" s="10" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C4" s="10" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>167</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O14" t="s">
+        <v>281</v>
       </c>
     </row>
   </sheetData>
@@ -4951,13 +5858,14 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="64.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -4971,28 +5879,37 @@
         <v>157</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C2" s="10" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C3" s="10" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>99</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>288</v>
       </c>
     </row>
   </sheetData>
@@ -5002,10 +5919,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC43BC44-11EE-4A7A-97EC-4F990AD9F102}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5015,28 +5932,236 @@
         <v>155</v>
       </c>
       <c r="B1" t="s">
-        <v>214</v>
+        <v>299</v>
       </c>
       <c r="C1" t="s">
-        <v>157</v>
+        <v>300</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
+      <c r="B2" s="11" t="s">
+        <v>313</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>301</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
+      <c r="B3" s="12" t="s">
+        <v>312</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>315</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
+      <c r="B4" s="14" t="s">
+        <v>311</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>310</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>332</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>333</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>334</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>335</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>336</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>4</v>
+      </c>
+      <c r="C13" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>3</v>
+      </c>
+      <c r="C16" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>4</v>
+      </c>
+      <c r="C17" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>3</v>
+      </c>
+      <c r="C20" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>4</v>
+      </c>
+      <c r="C21" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>27</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5051,7 +6176,7 @@
   <cols>
     <col min="1" max="1" width="4.33203125" customWidth="1"/>
     <col min="2" max="2" width="22.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.5546875" bestFit="1" customWidth="1"/>
@@ -5142,10 +6267,10 @@
         <v>131</v>
       </c>
       <c r="C2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E2" t="s">
         <v>159</v>
@@ -5181,7 +6306,7 @@
         <v>20</v>
       </c>
       <c r="P2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
@@ -5281,7 +6406,7 @@
         <v>15</v>
       </c>
       <c r="P4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.3">
@@ -5331,7 +6456,7 @@
         <v>12</v>
       </c>
       <c r="P5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.3">
@@ -5381,7 +6506,7 @@
         <v>10</v>
       </c>
       <c r="P6" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.3">
@@ -5431,7 +6556,7 @@
         <v>12</v>
       </c>
       <c r="P7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.3">
@@ -5442,10 +6567,10 @@
         <v>16</v>
       </c>
       <c r="C8" t="s">
+        <v>256</v>
+      </c>
+      <c r="D8" t="s">
         <v>257</v>
-      </c>
-      <c r="D8" t="s">
-        <v>258</v>
       </c>
       <c r="E8" t="s">
         <v>159</v>
@@ -5460,7 +6585,7 @@
         <v>160</v>
       </c>
       <c r="I8" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="K8" t="s">
         <v>175</v>
@@ -5478,7 +6603,7 @@
         <v>12</v>
       </c>
       <c r="P8" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.3">
@@ -5489,10 +6614,10 @@
         <v>134</v>
       </c>
       <c r="C9" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E9" t="s">
         <v>159</v>
@@ -5528,7 +6653,7 @@
         <v>14</v>
       </c>
       <c r="P9" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.3">
@@ -5539,10 +6664,10 @@
         <v>135</v>
       </c>
       <c r="C10" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D10" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E10" t="s">
         <v>158</v>
@@ -5589,10 +6714,10 @@
         <v>136</v>
       </c>
       <c r="C11" t="s">
+        <v>261</v>
+      </c>
+      <c r="D11" t="s">
         <v>262</v>
-      </c>
-      <c r="D11" t="s">
-        <v>263</v>
       </c>
       <c r="E11" t="s">
         <v>160</v>
@@ -5636,13 +6761,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>263</v>
+      </c>
+      <c r="C12" t="s">
         <v>264</v>
       </c>
-      <c r="C12" t="s">
-        <v>265</v>
-      </c>
       <c r="D12" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E12" t="s">
         <v>160</v>
@@ -5689,7 +6814,7 @@
         <v>137</v>
       </c>
       <c r="C13" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D13" t="s">
         <v>179</v>
@@ -5707,7 +6832,7 @@
         <v>163</v>
       </c>
       <c r="I13" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="J13" t="s">
         <v>99</v>
@@ -5728,7 +6853,7 @@
         <v>20</v>
       </c>
       <c r="P13" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.3">

</xml_diff>